<commit_message>
reran preg simulations for finer solutions
</commit_message>
<xml_diff>
--- a/tables/plasma_and_tissueBERs.xlsx
+++ b/tables/plasma_and_tissueBERs.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="219">
   <si>
     <t xml:space="preserve">dtxsid</t>
   </si>
@@ -53,27 +53,27 @@
     <t xml:space="preserve">2,2'-Methylenebis(ethyl-6-tert-butylphenol)</t>
   </si>
   <si>
+    <t xml:space="preserve">Cthyroid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maternal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thyroid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTXSID5020233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ergocalciferol</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cfthyroid</t>
   </si>
   <si>
     <t xml:space="preserve">fetal</t>
   </si>
   <si>
-    <t xml:space="preserve">thyroid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTXSID5020233</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ergocalciferol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cthyroid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maternal</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID4026684</t>
   </si>
   <si>
@@ -104,18 +104,24 @@
     <t xml:space="preserve">Bisphenol A diglycidyl ether</t>
   </si>
   <si>
+    <t xml:space="preserve">DTXSID8037752</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diphenyl isophthalate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cconceptus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conceptus</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTXSID0047246</t>
   </si>
   <si>
     <t xml:space="preserve">Darbufelone mesylate</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID8037752</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diphenyl isophthalate</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID7029241</t>
   </si>
   <si>
@@ -128,12 +134,6 @@
     <t xml:space="preserve">Sodium 2-mercaptobenzothiolate</t>
   </si>
   <si>
-    <t xml:space="preserve">Cconceptus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conceptus</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID2034881</t>
   </si>
   <si>
@@ -146,6 +146,12 @@
     <t xml:space="preserve">Nordihydroguaiaretic acid</t>
   </si>
   <si>
+    <t xml:space="preserve">DTXSID7025429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-Hydroxy-2-naphthyl disulfide</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTXSID7022253</t>
   </si>
   <si>
@@ -158,6 +164,15 @@
     <t xml:space="preserve">Morin hydrate</t>
   </si>
   <si>
+    <t xml:space="preserve">Cfliver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTXSID1026081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,3',5,5'-Tetrabromobisphenol A</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTXSID4023412</t>
   </si>
   <si>
@@ -170,27 +185,12 @@
     <t xml:space="preserve">Mepanipyrim</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID7025429</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6-Hydroxy-2-naphthyl disulfide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cfliver</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID5021097</t>
   </si>
   <si>
     <t xml:space="preserve">Oxytetracycline hydrochloride</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID1026081</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,3',5,5'-Tetrabromobisphenol A</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID6032514</t>
   </si>
   <si>
@@ -203,18 +203,18 @@
     <t xml:space="preserve">brain</t>
   </si>
   <si>
+    <t xml:space="preserve">DTXSID4034609</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fipronil</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTXSID9048196</t>
   </si>
   <si>
     <t xml:space="preserve">4-tert-Butylbenzenethiol</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID4034609</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fipronil</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID5044784</t>
   </si>
   <si>
@@ -245,12 +245,42 @@
     <t xml:space="preserve">Dichlone</t>
   </si>
   <si>
+    <t xml:space="preserve">DTXSID0047377</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVE6324</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTXSID4022523</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heptyl p-hydroxybenzoate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTXSID8029157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha-Amyl cinnamaldehyde</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTXSID1020807</t>
   </si>
   <si>
     <t xml:space="preserve">2-Mercaptobenzothiazole</t>
   </si>
   <si>
+    <t xml:space="preserve">DTXSID0020319</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorothalonil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTXSID5020366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyproterone acetate</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTXSID1034260</t>
   </si>
   <si>
@@ -263,28 +293,16 @@
     <t xml:space="preserve">Fenoxaprop-ethyl</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID0020319</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chlorothalonil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTXSID4022523</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heptyl p-hydroxybenzoate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTXSID8029157</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alpha-Amyl cinnamaldehyde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTXSID5020366</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyproterone acetate</t>
+    <t xml:space="preserve">DTXSID4027608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terbutylazine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTXSID4020870</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,2'-Methylenebis(4-methyl-6-tert-butylphenol)</t>
   </si>
   <si>
     <t xml:space="preserve">DTXSID4027236</t>
@@ -293,24 +311,12 @@
     <t xml:space="preserve">2,3-Dinitrotoluene</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID0047377</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVE6324</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID1020770</t>
   </si>
   <si>
     <t xml:space="preserve">Kepone</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID4020870</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,2'-Methylenebis(4-methyl-6-tert-butylphenol)</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID5021209</t>
   </si>
   <si>
@@ -323,6 +329,12 @@
     <t xml:space="preserve">Triflumizole</t>
   </si>
   <si>
+    <t xml:space="preserve">DTXSID3041663</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benzyl cinnamate</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTXSID7023645</t>
   </si>
   <si>
@@ -347,18 +359,6 @@
     <t xml:space="preserve">1,2-Dinitrobenzene</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID4027608</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terbutylazine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTXSID3041663</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benzyl cinnamate</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID7031248</t>
   </si>
   <si>
@@ -395,24 +395,30 @@
     <t xml:space="preserve">6-Methyl-2-thiouracil</t>
   </si>
   <si>
+    <t xml:space="preserve">DTXSID7032345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorhexidine diacetate</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTXSID7021239</t>
   </si>
   <si>
     <t xml:space="preserve">Retinoic acid</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID7032345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chlorhexidine diacetate</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID9047338</t>
   </si>
   <si>
     <t xml:space="preserve">HMR1426</t>
   </si>
   <si>
+    <t xml:space="preserve">DTXSID7032551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fluazinam</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTXSID8035180</t>
   </si>
   <si>
@@ -437,18 +443,18 @@
     <t xml:space="preserve">Mesotrione</t>
   </si>
   <si>
+    <t xml:space="preserve">DTXSID1023990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyanazine</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTXSID8047262</t>
   </si>
   <si>
     <t xml:space="preserve">CI-1029</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID7032551</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluazinam</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID3041409</t>
   </si>
   <si>
@@ -461,28 +467,40 @@
     <t xml:space="preserve">Fluoxastrobin</t>
   </si>
   <si>
+    <t xml:space="preserve">DTXSID1047310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farglitazar</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTXSID6034186</t>
   </si>
   <si>
     <t xml:space="preserve">Spironolactone</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID1023990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyanazine</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID2032348</t>
   </si>
   <si>
     <t xml:space="preserve">Chlorophacinone</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID1047310</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Farglitazar</t>
+    <t xml:space="preserve">DTXSID3023556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retinol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTXSID9020112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atrazine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTXSID9048190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methyl abietate</t>
   </si>
   <si>
     <t xml:space="preserve">DTXSID3047342</t>
@@ -497,30 +515,12 @@
     <t xml:space="preserve">Pirimicarb</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID3023556</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retinol</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID3021483</t>
   </si>
   <si>
     <t xml:space="preserve">Phenylacetaldehyde</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID9020112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atrazine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTXSID9048190</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Methyl abietate</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID1047368</t>
   </si>
   <si>
@@ -533,40 +533,52 @@
     <t xml:space="preserve">Disodium 4,4'-bis(2-sulfostyryl)biphenyl</t>
   </si>
   <si>
+    <t xml:space="preserve">DTXSID4020450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dicofol</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTXSID5041273</t>
   </si>
   <si>
     <t xml:space="preserve">Pyrazolone T</t>
   </si>
   <si>
+    <t xml:space="preserve">DTXSID0047371</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AVE5638</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTXSID1040794</t>
   </si>
   <si>
     <t xml:space="preserve">Sodium 2-phenylphenate tetrahydrate</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID4020450</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dicofol</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID2034598</t>
   </si>
   <si>
     <t xml:space="preserve">Fenoxaprop-P-ethyl</t>
   </si>
   <si>
+    <t xml:space="preserve">DTXSID4034528</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diclosulam</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTXSID5047295</t>
   </si>
   <si>
     <t xml:space="preserve">UK-373911</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID4034528</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diclosulam</t>
+    <t xml:space="preserve">DTXSID1034210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prodiamine</t>
   </si>
   <si>
     <t xml:space="preserve">DTXSID0034192</t>
@@ -587,10 +599,10 @@
     <t xml:space="preserve">1-Phenyl-2-nitropropene</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID1034210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prodiamine</t>
+    <t xml:space="preserve">DTXSID0021256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sulfasalazine</t>
   </si>
   <si>
     <t xml:space="preserve">DTXSID6041682</t>
@@ -599,18 +611,6 @@
     <t xml:space="preserve">Bromophenol blue</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID0047371</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AVE5638</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DTXSID0021256</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sulfasalazine</t>
-  </si>
-  <si>
     <t xml:space="preserve">DTXSID1032484</t>
   </si>
   <si>
@@ -629,16 +629,22 @@
     <t xml:space="preserve">Z-Tetrachlorvinphos</t>
   </si>
   <si>
+    <t xml:space="preserve">DTXSID0032572</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prallethrin</t>
+  </si>
+  <si>
     <t xml:space="preserve">DTXSID8020620</t>
   </si>
   <si>
     <t xml:space="preserve">Fenthion</t>
   </si>
   <si>
-    <t xml:space="preserve">DTXSID0032572</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prallethrin</t>
+    <t xml:space="preserve">DTXSID7022413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isoeugenol</t>
   </si>
   <si>
     <t xml:space="preserve">DTXSID5020944</t>
@@ -1037,7 +1043,7 @@
         <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>-2.74</v>
+        <v>-0.61</v>
       </c>
       <c r="D2"/>
       <c r="E2"/>
@@ -1066,7 +1072,7 @@
         <v>17</v>
       </c>
       <c r="C3" t="n">
-        <v>4.69</v>
+        <v>0.6</v>
       </c>
       <c r="D3" t="n">
         <v>-1.21</v>
@@ -1082,10 +1088,10 @@
         <v>-2.45</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K3" t="s">
         <v>15</v>
@@ -1099,7 +1105,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="n">
-        <v>4.69</v>
+        <v>0.6</v>
       </c>
       <c r="D4" t="n">
         <v>-1.21</v>
@@ -1115,10 +1121,10 @@
         <v>-2.45</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K4" t="s">
         <v>15</v>
@@ -1132,18 +1138,18 @@
         <v>21</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.28</v>
+        <v>-0.36</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="n">
-        <v>0.23</v>
+        <v>0.12</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.61</v>
+        <v>-0.72</v>
       </c>
       <c r="G5"/>
       <c r="H5" t="n">
-        <v>-0.61</v>
+        <v>-0.72</v>
       </c>
       <c r="I5" t="s">
         <v>13</v>
@@ -1163,26 +1169,26 @@
         <v>23</v>
       </c>
       <c r="C6" t="n">
-        <v>0.11</v>
+        <v>0.07</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.49</v>
+        <v>-0.66</v>
       </c>
       <c r="E6" t="n">
-        <v>1.84</v>
+        <v>1.71</v>
       </c>
       <c r="F6" t="n">
-        <v>1.15</v>
+        <v>1.02</v>
       </c>
       <c r="G6"/>
       <c r="H6" t="n">
-        <v>-0.49</v>
+        <v>-0.66</v>
       </c>
       <c r="I6" t="s">
         <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K6" t="s">
         <v>25</v>
@@ -1196,7 +1202,7 @@
         <v>27</v>
       </c>
       <c r="C7" t="n">
-        <v>5.73</v>
+        <v>2.76</v>
       </c>
       <c r="D7"/>
       <c r="E7"/>
@@ -1208,10 +1214,10 @@
         <v>-0.04</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K7" t="s">
         <v>15</v>
@@ -1225,7 +1231,7 @@
         <v>29</v>
       </c>
       <c r="C8" t="n">
-        <v>1.17</v>
+        <v>0.09</v>
       </c>
       <c r="D8" t="n">
         <v>0.27</v>
@@ -1244,7 +1250,7 @@
         <v>24</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K8" t="s">
         <v>25</v>
@@ -1258,71 +1264,71 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.81</v>
-      </c>
+        <v>0.28</v>
+      </c>
+      <c r="D9"/>
       <c r="E9" t="n">
-        <v>2.52</v>
+        <v>0.63</v>
       </c>
       <c r="F9" t="n">
-        <v>2.27</v>
+        <v>0.91</v>
       </c>
       <c r="G9"/>
       <c r="H9" t="n">
-        <v>0.81</v>
+        <v>0.63</v>
       </c>
       <c r="I9" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="K9" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C10" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="D10"/>
+        <v>0.32</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.76</v>
+      </c>
       <c r="E10" t="n">
-        <v>0.85</v>
+        <v>2.47</v>
       </c>
       <c r="F10" t="n">
-        <v>1.12</v>
+        <v>2.22</v>
       </c>
       <c r="G10"/>
       <c r="H10" t="n">
-        <v>0.85</v>
+        <v>0.76</v>
       </c>
       <c r="I10" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J10" t="s">
         <v>14</v>
       </c>
       <c r="K10" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C11" t="n">
-        <v>2.14</v>
+        <v>0.98</v>
       </c>
       <c r="D11"/>
       <c r="E11"/>
@@ -1336,10 +1342,10 @@
         <v>1.08</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K11" t="s">
         <v>15</v>
@@ -1347,13 +1353,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C12" t="n">
-        <v>1.38</v>
+        <v>0.31</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
@@ -1365,13 +1371,13 @@
         <v>1.21</v>
       </c>
       <c r="I12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13">
@@ -1382,24 +1388,24 @@
         <v>41</v>
       </c>
       <c r="C13" t="n">
-        <v>1.1</v>
+        <v>2.78</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="n">
         <v>2.24</v>
       </c>
       <c r="F13" t="n">
-        <v>1.29</v>
+        <v>1.28</v>
       </c>
       <c r="G13"/>
       <c r="H13" t="n">
-        <v>1.29</v>
+        <v>1.28</v>
       </c>
       <c r="I13" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J13" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K13" t="s">
         <v>15</v>
@@ -1413,7 +1419,7 @@
         <v>43</v>
       </c>
       <c r="C14" t="n">
-        <v>2.46</v>
+        <v>1.03</v>
       </c>
       <c r="D14" t="n">
         <v>2.93</v>
@@ -1429,10 +1435,10 @@
         <v>1.56</v>
       </c>
       <c r="I14" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J14" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K14" t="s">
         <v>15</v>
@@ -1446,27 +1452,29 @@
         <v>45</v>
       </c>
       <c r="C15" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="D15"/>
+        <v>1.6</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1.56</v>
+      </c>
       <c r="E15" t="n">
-        <v>1.61</v>
+        <v>3.01</v>
       </c>
       <c r="F15" t="n">
-        <v>1.64</v>
+        <v>2.2</v>
       </c>
       <c r="G15"/>
       <c r="H15" t="n">
-        <v>1.61</v>
+        <v>1.56</v>
       </c>
       <c r="I15" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J15" t="s">
         <v>14</v>
       </c>
       <c r="K15" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16">
@@ -1477,27 +1485,27 @@
         <v>47</v>
       </c>
       <c r="C16" t="n">
-        <v>2.46</v>
-      </c>
-      <c r="D16" t="n">
-        <v>1.65</v>
-      </c>
-      <c r="E16"/>
+        <v>3.3</v>
+      </c>
+      <c r="D16"/>
+      <c r="E16" t="n">
+        <v>1.6</v>
+      </c>
       <c r="F16" t="n">
-        <v>2.95</v>
+        <v>1.64</v>
       </c>
       <c r="G16"/>
       <c r="H16" t="n">
-        <v>1.65</v>
+        <v>1.6</v>
       </c>
       <c r="I16" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J16" t="s">
         <v>19</v>
       </c>
       <c r="K16" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17">
@@ -1508,24 +1516,24 @@
         <v>49</v>
       </c>
       <c r="C17" t="n">
-        <v>2.17</v>
+        <v>3.42</v>
       </c>
       <c r="D17" t="n">
-        <v>1.8</v>
+        <v>1.65</v>
       </c>
       <c r="E17"/>
       <c r="F17" t="n">
-        <v>2.52</v>
+        <v>2.95</v>
       </c>
       <c r="G17"/>
       <c r="H17" t="n">
-        <v>1.8</v>
+        <v>1.65</v>
       </c>
       <c r="I17" t="s">
         <v>24</v>
       </c>
       <c r="J17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K17" t="s">
         <v>25</v>
@@ -1533,92 +1541,92 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" t="n">
-        <v>1.57</v>
-      </c>
-      <c r="D18"/>
-      <c r="E18" t="n">
-        <v>2.79</v>
-      </c>
+        <v>3.42</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="E18"/>
       <c r="F18" t="n">
-        <v>1.84</v>
+        <v>2.95</v>
       </c>
       <c r="G18"/>
       <c r="H18" t="n">
-        <v>1.84</v>
+        <v>1.65</v>
       </c>
       <c r="I18" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="J18" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K18" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
         <v>52</v>
       </c>
-      <c r="B19" t="s">
-        <v>53</v>
-      </c>
       <c r="C19" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1.88</v>
-      </c>
+        <v>1.39</v>
+      </c>
+      <c r="D19"/>
       <c r="E19" t="n">
-        <v>3.29</v>
+        <v>1.85</v>
       </c>
       <c r="F19" t="n">
-        <v>2.48</v>
+        <v>1.74</v>
       </c>
       <c r="G19"/>
       <c r="H19" t="n">
-        <v>1.88</v>
+        <v>1.74</v>
       </c>
       <c r="I19" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="J19" t="s">
         <v>14</v>
       </c>
       <c r="K19" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C20" t="n">
-        <v>2.49</v>
+        <v>1.33</v>
       </c>
       <c r="D20" t="n">
-        <v>1.98</v>
+        <v>1.8</v>
       </c>
       <c r="E20"/>
-      <c r="F20"/>
+      <c r="F20" t="n">
+        <v>2.52</v>
+      </c>
       <c r="G20"/>
       <c r="H20" t="n">
-        <v>1.98</v>
+        <v>1.8</v>
       </c>
       <c r="I20" t="s">
         <v>24</v>
       </c>
       <c r="J20" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K20" t="s">
         <v>25</v>
@@ -1626,30 +1634,30 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C21" t="n">
-        <v>2.22</v>
+        <v>2.52</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="n">
-        <v>2.1</v>
+        <v>2.76</v>
       </c>
       <c r="F21" t="n">
-        <v>1.99</v>
+        <v>1.81</v>
       </c>
       <c r="G21"/>
       <c r="H21" t="n">
-        <v>1.99</v>
+        <v>1.81</v>
       </c>
       <c r="I21" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J21" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K21" t="s">
         <v>15</v>
@@ -1657,90 +1665,90 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C22" t="n">
-        <v>2.54</v>
-      </c>
-      <c r="D22"/>
-      <c r="E22" t="n">
-        <v>3.21</v>
-      </c>
-      <c r="F22" t="n">
-        <v>2.01</v>
-      </c>
+        <v>1.5</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="E22"/>
+      <c r="F22"/>
       <c r="G22"/>
       <c r="H22" t="n">
-        <v>2.01</v>
+        <v>1.98</v>
       </c>
       <c r="I22" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="J22" t="s">
         <v>14</v>
       </c>
       <c r="K22" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C23" t="n">
-        <v>2.76</v>
-      </c>
-      <c r="D23" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="E23"/>
-      <c r="F23"/>
+        <v>0.85</v>
+      </c>
+      <c r="D23"/>
+      <c r="E23" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2.01</v>
+      </c>
       <c r="G23"/>
       <c r="H23" t="n">
-        <v>2.05</v>
+        <v>2.01</v>
       </c>
       <c r="I23" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="J23" t="s">
         <v>19</v>
       </c>
       <c r="K23" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C24" t="n">
-        <v>2.11</v>
+        <v>2.82</v>
       </c>
       <c r="D24"/>
       <c r="E24" t="n">
-        <v>3.47</v>
+        <v>3.46</v>
       </c>
       <c r="F24" t="n">
-        <v>2.07</v>
+        <v>2.05</v>
       </c>
       <c r="G24"/>
       <c r="H24" t="n">
-        <v>2.07</v>
+        <v>2.05</v>
       </c>
       <c r="I24" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J24" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K24" t="s">
         <v>15</v>
@@ -1748,90 +1756,90 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C25" t="n">
-        <v>3.09</v>
-      </c>
-      <c r="D25"/>
-      <c r="E25" t="n">
-        <v>2.35</v>
-      </c>
-      <c r="F25" t="n">
-        <v>2.09</v>
-      </c>
+        <v>2.23</v>
+      </c>
+      <c r="D25" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="E25"/>
+      <c r="F25"/>
       <c r="G25"/>
       <c r="H25" t="n">
-        <v>2.09</v>
+        <v>2.05</v>
       </c>
       <c r="I25" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J25" t="s">
         <v>14</v>
       </c>
       <c r="K25" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C26" t="n">
-        <v>2.29</v>
-      </c>
-      <c r="D26" t="n">
-        <v>2.25</v>
-      </c>
+        <v>1.5</v>
+      </c>
+      <c r="D26"/>
       <c r="E26" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="F26"/>
+        <v>2.35</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2.09</v>
+      </c>
       <c r="G26"/>
       <c r="H26" t="n">
-        <v>2.25</v>
+        <v>2.09</v>
       </c>
       <c r="I26" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J26" t="s">
         <v>19</v>
       </c>
       <c r="K26" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C27" t="n">
-        <v>3.18</v>
+        <v>3.45</v>
       </c>
       <c r="D27" t="n">
-        <v>2.28</v>
-      </c>
-      <c r="E27"/>
+        <v>2.24</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2.6</v>
+      </c>
       <c r="F27"/>
       <c r="G27"/>
       <c r="H27" t="n">
-        <v>2.28</v>
+        <v>2.24</v>
       </c>
       <c r="I27" t="s">
         <v>24</v>
       </c>
       <c r="J27" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K27" t="s">
         <v>25</v>
@@ -1839,28 +1847,28 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C28" t="n">
-        <v>3.1</v>
+        <v>3.5</v>
       </c>
       <c r="D28" t="n">
-        <v>2.52</v>
+        <v>2.26</v>
       </c>
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28"/>
       <c r="H28" t="n">
-        <v>2.52</v>
+        <v>2.26</v>
       </c>
       <c r="I28" t="s">
         <v>24</v>
       </c>
       <c r="J28" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K28" t="s">
         <v>25</v>
@@ -1868,23 +1876,19 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C29" t="n">
-        <v>2.92</v>
+        <v>2.36</v>
       </c>
       <c r="D29" t="n">
         <v>2.52</v>
       </c>
-      <c r="E29" t="n">
-        <v>3.11</v>
-      </c>
-      <c r="F29" t="n">
-        <v>2.64</v>
-      </c>
+      <c r="E29"/>
+      <c r="F29"/>
       <c r="G29"/>
       <c r="H29" t="n">
         <v>2.52</v>
@@ -1893,7 +1897,7 @@
         <v>24</v>
       </c>
       <c r="J29" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K29" t="s">
         <v>25</v>
@@ -1901,27 +1905,29 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C30" t="n">
-        <v>3.08</v>
+        <v>1.99</v>
       </c>
       <c r="D30" t="n">
-        <v>2.59</v>
+        <v>2.52</v>
       </c>
       <c r="E30" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="F30"/>
+        <v>3.11</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2.64</v>
+      </c>
       <c r="G30"/>
       <c r="H30" t="n">
-        <v>2.59</v>
+        <v>2.52</v>
       </c>
       <c r="I30" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="J30" t="s">
         <v>14</v>
@@ -1932,55 +1938,51 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C31" t="n">
-        <v>3.26</v>
-      </c>
-      <c r="D31" t="n">
-        <v>2.66</v>
-      </c>
-      <c r="E31" t="n">
-        <v>4.02</v>
-      </c>
+        <v>2.05</v>
+      </c>
+      <c r="D31"/>
+      <c r="E31"/>
       <c r="F31" t="n">
-        <v>3.24</v>
+        <v>2.54</v>
       </c>
       <c r="G31"/>
       <c r="H31" t="n">
-        <v>2.66</v>
+        <v>2.54</v>
       </c>
       <c r="I31" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="J31" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K31" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C32" t="n">
-        <v>2.38</v>
+        <v>2.65</v>
       </c>
       <c r="D32"/>
       <c r="E32"/>
-      <c r="F32" t="n">
-        <v>2.66</v>
-      </c>
-      <c r="G32"/>
+      <c r="F32"/>
+      <c r="G32" t="n">
+        <v>2.57</v>
+      </c>
       <c r="H32" t="n">
-        <v>2.66</v>
+        <v>2.57</v>
       </c>
       <c r="I32" t="s">
         <v>13</v>
@@ -1994,30 +1996,28 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C33" t="n">
-        <v>2.96</v>
+        <v>2.73</v>
       </c>
       <c r="D33"/>
-      <c r="E33" t="n">
-        <v>3.72</v>
-      </c>
+      <c r="E33"/>
       <c r="F33" t="n">
-        <v>2.69</v>
+        <v>2.58</v>
       </c>
       <c r="G33"/>
       <c r="H33" t="n">
-        <v>2.69</v>
+        <v>2.58</v>
       </c>
       <c r="I33" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J33" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K33" t="s">
         <v>15</v>
@@ -2025,51 +2025,55 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C34" t="n">
-        <v>3.14</v>
-      </c>
-      <c r="D34"/>
-      <c r="E34"/>
+        <v>2.27</v>
+      </c>
+      <c r="D34" t="n">
+        <v>2.59</v>
+      </c>
+      <c r="E34" t="n">
+        <v>3.5</v>
+      </c>
       <c r="F34"/>
-      <c r="G34" t="n">
-        <v>2.8</v>
-      </c>
+      <c r="G34"/>
       <c r="H34" t="n">
-        <v>2.8</v>
+        <v>2.59</v>
       </c>
       <c r="I34" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="J34" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K34" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C35" t="n">
-        <v>3.06</v>
+        <v>2.96</v>
       </c>
       <c r="D35"/>
-      <c r="E35"/>
+      <c r="E35" t="n">
+        <v>3.63</v>
+      </c>
       <c r="F35" t="n">
-        <v>2.8</v>
+        <v>2.6</v>
       </c>
       <c r="G35"/>
       <c r="H35" t="n">
-        <v>2.8</v>
+        <v>2.6</v>
       </c>
       <c r="I35" t="s">
         <v>13</v>
@@ -2083,22 +2087,22 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C36" t="n">
-        <v>2.95</v>
+        <v>2.43</v>
       </c>
       <c r="D36"/>
       <c r="E36"/>
       <c r="F36" t="n">
-        <v>2.81</v>
+        <v>2.61</v>
       </c>
       <c r="G36"/>
       <c r="H36" t="n">
-        <v>2.81</v>
+        <v>2.61</v>
       </c>
       <c r="I36" t="s">
         <v>13</v>
@@ -2112,59 +2116,61 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B37" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C37" t="n">
-        <v>3.63</v>
-      </c>
-      <c r="D37"/>
+        <v>2.18</v>
+      </c>
+      <c r="D37" t="n">
+        <v>2.66</v>
+      </c>
       <c r="E37" t="n">
-        <v>3.05</v>
+        <v>4.02</v>
       </c>
       <c r="F37" t="n">
-        <v>2.83</v>
+        <v>3.24</v>
       </c>
       <c r="G37"/>
       <c r="H37" t="n">
-        <v>2.83</v>
+        <v>2.66</v>
       </c>
       <c r="I37" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="J37" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="K37" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C38" t="n">
-        <v>3.07</v>
+        <v>4.05</v>
       </c>
       <c r="D38"/>
       <c r="E38"/>
       <c r="F38" t="n">
-        <v>2.84</v>
+        <v>2.66</v>
       </c>
       <c r="G38"/>
       <c r="H38" t="n">
-        <v>2.84</v>
+        <v>2.66</v>
       </c>
       <c r="I38" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J38" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K38" t="s">
         <v>15</v>
@@ -2172,28 +2178,22 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C39" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="D39" t="n">
-        <v>3.42</v>
-      </c>
-      <c r="E39" t="n">
-        <v>3.69</v>
-      </c>
+        <v>2.64</v>
+      </c>
+      <c r="D39"/>
+      <c r="E39"/>
       <c r="F39" t="n">
-        <v>2.88</v>
-      </c>
-      <c r="G39" t="n">
-        <v>3.92</v>
-      </c>
+        <v>2.78</v>
+      </c>
+      <c r="G39"/>
       <c r="H39" t="n">
-        <v>2.88</v>
+        <v>2.78</v>
       </c>
       <c r="I39" t="s">
         <v>13</v>
@@ -2207,24 +2207,24 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C40" t="n">
-        <v>3.47</v>
+        <v>3.15</v>
       </c>
       <c r="D40"/>
       <c r="E40"/>
       <c r="F40" t="n">
-        <v>2.88</v>
+        <v>2.79</v>
       </c>
       <c r="G40" t="n">
-        <v>3.22</v>
+        <v>3.14</v>
       </c>
       <c r="H40" t="n">
-        <v>2.88</v>
+        <v>2.79</v>
       </c>
       <c r="I40" t="s">
         <v>13</v>
@@ -2238,92 +2238,94 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C41" t="n">
-        <v>3.67</v>
-      </c>
-      <c r="D41" t="n">
-        <v>2.89</v>
-      </c>
-      <c r="E41"/>
-      <c r="F41"/>
+        <v>1.75</v>
+      </c>
+      <c r="D41"/>
+      <c r="E41" t="n">
+        <v>3.05</v>
+      </c>
+      <c r="F41" t="n">
+        <v>2.83</v>
+      </c>
       <c r="G41"/>
       <c r="H41" t="n">
-        <v>2.89</v>
+        <v>2.83</v>
       </c>
       <c r="I41" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J41" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="K41" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C42" t="n">
-        <v>2.44</v>
+        <v>4.33</v>
       </c>
       <c r="D42" t="n">
-        <v>3.19</v>
+        <v>3.41</v>
       </c>
       <c r="E42" t="n">
-        <v>2.99</v>
+        <v>3.69</v>
       </c>
       <c r="F42" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="G42"/>
+        <v>2.88</v>
+      </c>
+      <c r="G42" t="n">
+        <v>3.92</v>
+      </c>
       <c r="H42" t="n">
-        <v>2.9</v>
+        <v>2.88</v>
       </c>
       <c r="I42" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="J42" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="K42" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C43" t="n">
-        <v>3.84</v>
+        <v>2.73</v>
       </c>
       <c r="D43" t="n">
-        <v>2.97</v>
+        <v>2.89</v>
       </c>
       <c r="E43"/>
-      <c r="F43" t="n">
-        <v>3.67</v>
-      </c>
+      <c r="F43"/>
       <c r="G43"/>
       <c r="H43" t="n">
-        <v>2.97</v>
+        <v>2.89</v>
       </c>
       <c r="I43" t="s">
         <v>24</v>
       </c>
       <c r="J43" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K43" t="s">
         <v>25</v>
@@ -2331,57 +2333,63 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B44" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C44" t="n">
-        <v>3.93</v>
+        <v>1.91</v>
       </c>
       <c r="D44" t="n">
-        <v>2.97</v>
-      </c>
-      <c r="E44"/>
-      <c r="F44"/>
+        <v>3.19</v>
+      </c>
+      <c r="E44" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="F44" t="n">
+        <v>2.9</v>
+      </c>
       <c r="G44"/>
       <c r="H44" t="n">
-        <v>2.97</v>
+        <v>2.9</v>
       </c>
       <c r="I44" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J44" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="K44" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C45" t="n">
-        <v>4.2</v>
+        <v>2.77</v>
       </c>
       <c r="D45"/>
-      <c r="E45"/>
+      <c r="E45" t="n">
+        <v>3.32</v>
+      </c>
       <c r="F45" t="n">
-        <v>3.04</v>
+        <v>2.9</v>
       </c>
       <c r="G45"/>
       <c r="H45" t="n">
-        <v>3.04</v>
+        <v>2.9</v>
       </c>
       <c r="I45" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J45" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K45" t="s">
         <v>15</v>
@@ -2389,92 +2397,88 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B46" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C46" t="n">
-        <v>3.17</v>
-      </c>
-      <c r="D46"/>
-      <c r="E46" t="n">
-        <v>3.22</v>
-      </c>
+        <v>2.57</v>
+      </c>
+      <c r="D46" t="n">
+        <v>2.97</v>
+      </c>
+      <c r="E46"/>
       <c r="F46" t="n">
-        <v>3.04</v>
-      </c>
-      <c r="G46" t="n">
-        <v>3.4</v>
-      </c>
+        <v>3.67</v>
+      </c>
+      <c r="G46"/>
       <c r="H46" t="n">
-        <v>3.04</v>
+        <v>2.97</v>
       </c>
       <c r="I46" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="J46" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="K46" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C47" t="n">
-        <v>3.03</v>
-      </c>
-      <c r="D47"/>
+        <v>3.02</v>
+      </c>
+      <c r="D47" t="n">
+        <v>2.97</v>
+      </c>
       <c r="E47"/>
-      <c r="F47" t="n">
-        <v>3.08</v>
-      </c>
+      <c r="F47"/>
       <c r="G47"/>
       <c r="H47" t="n">
-        <v>3.08</v>
+        <v>2.97</v>
       </c>
       <c r="I47" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J47" t="s">
         <v>14</v>
       </c>
       <c r="K47" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C48" t="n">
-        <v>3.17</v>
+        <v>3.71</v>
       </c>
       <c r="D48"/>
-      <c r="E48" t="n">
-        <v>3.61</v>
-      </c>
+      <c r="E48"/>
       <c r="F48" t="n">
-        <v>3.19</v>
+        <v>3.04</v>
       </c>
       <c r="G48"/>
       <c r="H48" t="n">
-        <v>3.19</v>
+        <v>3.04</v>
       </c>
       <c r="I48" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J48" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K48" t="s">
         <v>15</v>
@@ -2482,243 +2486,247 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B49" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C49" t="n">
-        <v>3.32</v>
+        <v>2.15</v>
       </c>
       <c r="D49"/>
-      <c r="E49"/>
-      <c r="F49"/>
+      <c r="E49" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="F49" t="n">
+        <v>3.04</v>
+      </c>
       <c r="G49" t="n">
-        <v>3.25</v>
+        <v>3.4</v>
       </c>
       <c r="H49" t="n">
-        <v>3.25</v>
+        <v>3.04</v>
       </c>
       <c r="I49" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J49" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K49" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B50" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C50" t="n">
-        <v>3.64</v>
+        <v>2.26</v>
       </c>
       <c r="D50"/>
-      <c r="E50" t="n">
-        <v>3.99</v>
-      </c>
-      <c r="F50" t="n">
-        <v>3.37</v>
-      </c>
-      <c r="G50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50" t="n">
+        <v>3.25</v>
+      </c>
       <c r="H50" t="n">
-        <v>3.37</v>
+        <v>3.25</v>
       </c>
       <c r="I50" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J50" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K50" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B51" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C51" t="n">
-        <v>3.38</v>
+        <v>2.54</v>
       </c>
       <c r="D51"/>
-      <c r="E51"/>
+      <c r="E51" t="n">
+        <v>3.99</v>
+      </c>
       <c r="F51" t="n">
-        <v>3.38</v>
+        <v>3.37</v>
       </c>
       <c r="G51"/>
       <c r="H51" t="n">
-        <v>3.38</v>
+        <v>3.37</v>
       </c>
       <c r="I51" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J51" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K51" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B52" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C52" t="n">
-        <v>3.85</v>
-      </c>
-      <c r="D52" t="n">
-        <v>3.42</v>
-      </c>
-      <c r="E52" t="n">
-        <v>5.94</v>
-      </c>
+        <v>1.56</v>
+      </c>
+      <c r="D52"/>
+      <c r="E52"/>
       <c r="F52" t="n">
-        <v>5.73</v>
+        <v>3.38</v>
       </c>
       <c r="G52"/>
       <c r="H52" t="n">
-        <v>3.42</v>
+        <v>3.38</v>
       </c>
       <c r="I52" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J52" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="K52" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B53" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C53" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="D53" t="n">
         <v>3.42</v>
       </c>
-      <c r="D53"/>
       <c r="E53" t="n">
-        <v>3.43</v>
+        <v>5.94</v>
       </c>
       <c r="F53" t="n">
-        <v>3.43</v>
+        <v>5.73</v>
       </c>
       <c r="G53"/>
       <c r="H53" t="n">
-        <v>3.43</v>
+        <v>3.42</v>
       </c>
       <c r="I53" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="J53" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="K53" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B54" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C54" t="n">
-        <v>3.93</v>
-      </c>
-      <c r="D54" t="n">
-        <v>3.51</v>
-      </c>
-      <c r="E54"/>
-      <c r="F54"/>
+        <v>3.2</v>
+      </c>
+      <c r="D54"/>
+      <c r="E54" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="F54" t="n">
+        <v>3.43</v>
+      </c>
       <c r="G54"/>
       <c r="H54" t="n">
-        <v>3.51</v>
+        <v>3.43</v>
       </c>
       <c r="I54" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J54" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="K54" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B55" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C55" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="D55"/>
+        <v>3.56</v>
+      </c>
+      <c r="D55" t="n">
+        <v>3.51</v>
+      </c>
       <c r="E55"/>
-      <c r="F55" t="n">
-        <v>3.53</v>
-      </c>
+      <c r="F55"/>
       <c r="G55"/>
       <c r="H55" t="n">
-        <v>3.53</v>
+        <v>3.51</v>
       </c>
       <c r="I55" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J55" t="s">
         <v>14</v>
       </c>
       <c r="K55" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B56" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C56" t="n">
-        <v>2.25</v>
+        <v>3.61</v>
       </c>
       <c r="D56" t="n">
-        <v>3.77</v>
+        <v>3.75</v>
       </c>
       <c r="E56" t="n">
-        <v>4.22</v>
+        <v>4.2</v>
       </c>
       <c r="F56" t="n">
-        <v>3.53</v>
+        <v>3.51</v>
       </c>
       <c r="G56"/>
       <c r="H56" t="n">
-        <v>3.53</v>
+        <v>3.51</v>
       </c>
       <c r="I56" t="s">
         <v>61</v>
       </c>
       <c r="J56" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K56" t="s">
         <v>62</v>
@@ -2726,179 +2734,179 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B57" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C57" t="n">
-        <v>4.47</v>
-      </c>
-      <c r="D57" t="n">
-        <v>3.54</v>
-      </c>
+        <v>4.27</v>
+      </c>
+      <c r="D57"/>
       <c r="E57"/>
-      <c r="F57"/>
+      <c r="F57" t="n">
+        <v>3.53</v>
+      </c>
       <c r="G57"/>
       <c r="H57" t="n">
-        <v>3.54</v>
+        <v>3.53</v>
       </c>
       <c r="I57" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J57" t="s">
         <v>19</v>
       </c>
       <c r="K57" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B58" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C58" t="n">
-        <v>3.58</v>
-      </c>
-      <c r="D58"/>
+        <v>3.36</v>
+      </c>
+      <c r="D58" t="n">
+        <v>3.54</v>
+      </c>
       <c r="E58"/>
-      <c r="F58" t="n">
-        <v>3.63</v>
-      </c>
+      <c r="F58"/>
       <c r="G58"/>
       <c r="H58" t="n">
-        <v>3.63</v>
+        <v>3.54</v>
       </c>
       <c r="I58" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J58" t="s">
         <v>14</v>
       </c>
       <c r="K58" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B59" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C59" t="n">
-        <v>5.09</v>
-      </c>
-      <c r="D59" t="n">
-        <v>3.66</v>
-      </c>
-      <c r="E59"/>
-      <c r="F59"/>
+        <v>3.04</v>
+      </c>
+      <c r="D59"/>
+      <c r="E59" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="F59" t="n">
+        <v>3.61</v>
+      </c>
       <c r="G59"/>
       <c r="H59" t="n">
-        <v>3.66</v>
+        <v>3.61</v>
       </c>
       <c r="I59" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="J59" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K59" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B60" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C60" t="n">
-        <v>4.68</v>
-      </c>
-      <c r="D60" t="n">
-        <v>3.66</v>
-      </c>
-      <c r="E60" t="n">
-        <v>4.38</v>
-      </c>
+        <v>5.2</v>
+      </c>
+      <c r="D60"/>
+      <c r="E60"/>
       <c r="F60" t="n">
-        <v>5.05</v>
+        <v>3.63</v>
       </c>
       <c r="G60"/>
       <c r="H60" t="n">
-        <v>3.66</v>
+        <v>3.63</v>
       </c>
       <c r="I60" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J60" t="s">
         <v>19</v>
       </c>
       <c r="K60" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B61" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C61" t="n">
-        <v>3.59</v>
-      </c>
-      <c r="D61"/>
-      <c r="E61" t="n">
-        <v>3.81</v>
-      </c>
-      <c r="F61" t="n">
-        <v>3.76</v>
-      </c>
+        <v>2.62</v>
+      </c>
+      <c r="D61" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="E61"/>
+      <c r="F61"/>
       <c r="G61"/>
       <c r="H61" t="n">
-        <v>3.76</v>
+        <v>3.66</v>
       </c>
       <c r="I61" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="J61" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="K61" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B62" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C62" t="n">
-        <v>4.23</v>
+        <v>3.66</v>
       </c>
       <c r="D62" t="n">
-        <v>3.87</v>
-      </c>
-      <c r="E62"/>
-      <c r="F62"/>
+        <v>3.66</v>
+      </c>
+      <c r="E62" t="n">
+        <v>4.38</v>
+      </c>
+      <c r="F62" t="n">
+        <v>5.05</v>
+      </c>
       <c r="G62"/>
       <c r="H62" t="n">
-        <v>3.87</v>
+        <v>3.66</v>
       </c>
       <c r="I62" t="s">
         <v>24</v>
       </c>
       <c r="J62" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K62" t="s">
         <v>25</v>
@@ -2906,146 +2914,146 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B63" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C63" t="n">
-        <v>3.5</v>
+        <v>2.86</v>
       </c>
       <c r="D63"/>
       <c r="E63" t="n">
-        <v>3.89</v>
+        <v>3.81</v>
       </c>
       <c r="F63" t="n">
-        <v>3.89</v>
+        <v>3.76</v>
       </c>
       <c r="G63"/>
       <c r="H63" t="n">
-        <v>3.89</v>
+        <v>3.76</v>
       </c>
       <c r="I63" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="J63" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="K63" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B64" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C64" t="n">
-        <v>5.29</v>
-      </c>
-      <c r="D64" t="n">
-        <v>3.97</v>
-      </c>
+        <v>3.73</v>
+      </c>
+      <c r="D64"/>
       <c r="E64"/>
-      <c r="F64"/>
+      <c r="F64" t="n">
+        <v>3.86</v>
+      </c>
       <c r="G64"/>
       <c r="H64" t="n">
-        <v>3.97</v>
+        <v>3.86</v>
       </c>
       <c r="I64" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="J64" t="s">
         <v>14</v>
       </c>
       <c r="K64" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B65" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C65" t="n">
-        <v>4.33</v>
-      </c>
-      <c r="D65"/>
+        <v>3.31</v>
+      </c>
+      <c r="D65" t="n">
+        <v>3.87</v>
+      </c>
       <c r="E65"/>
-      <c r="F65" t="n">
-        <v>3.98</v>
-      </c>
+      <c r="F65"/>
       <c r="G65"/>
       <c r="H65" t="n">
-        <v>3.98</v>
+        <v>3.87</v>
       </c>
       <c r="I65" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J65" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K65" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B66" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C66" t="n">
-        <v>4.06</v>
-      </c>
-      <c r="D66"/>
-      <c r="E66" t="n">
-        <v>4.04</v>
-      </c>
+        <v>3.13</v>
+      </c>
+      <c r="D66" t="n">
+        <v>3.97</v>
+      </c>
+      <c r="E66"/>
       <c r="F66"/>
       <c r="G66"/>
       <c r="H66" t="n">
-        <v>4.04</v>
+        <v>3.97</v>
       </c>
       <c r="I66" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="J66" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="K66" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B67" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C67" t="n">
-        <v>3.96</v>
+        <v>3.5</v>
       </c>
       <c r="D67"/>
       <c r="E67"/>
       <c r="F67" t="n">
-        <v>4.08</v>
+        <v>3.98</v>
       </c>
       <c r="G67"/>
       <c r="H67" t="n">
-        <v>4.08</v>
+        <v>3.98</v>
       </c>
       <c r="I67" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J67" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K67" t="s">
         <v>15</v>
@@ -3053,142 +3061,140 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B68" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C68" t="n">
-        <v>3.31</v>
-      </c>
-      <c r="D68" t="n">
-        <v>4.12</v>
-      </c>
-      <c r="E68"/>
+        <v>3.74</v>
+      </c>
+      <c r="D68"/>
+      <c r="E68" t="n">
+        <v>4.01</v>
+      </c>
       <c r="F68"/>
       <c r="G68"/>
       <c r="H68" t="n">
-        <v>4.12</v>
+        <v>4.01</v>
       </c>
       <c r="I68" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="J68" t="s">
         <v>14</v>
       </c>
       <c r="K68" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B69" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C69" t="n">
-        <v>4.44</v>
+        <v>3.31</v>
       </c>
       <c r="D69"/>
       <c r="E69" t="n">
-        <v>4.2</v>
+        <v>4.04</v>
       </c>
       <c r="F69"/>
       <c r="G69"/>
       <c r="H69" t="n">
-        <v>4.2</v>
+        <v>4.04</v>
       </c>
       <c r="I69" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="J69" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="K69" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B70" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C70" t="n">
-        <v>5.05</v>
-      </c>
-      <c r="D70"/>
+        <v>5.98</v>
+      </c>
+      <c r="D70" t="n">
+        <v>4.11</v>
+      </c>
       <c r="E70"/>
-      <c r="F70" t="n">
-        <v>4.24</v>
-      </c>
+      <c r="F70"/>
       <c r="G70"/>
       <c r="H70" t="n">
-        <v>4.24</v>
+        <v>4.11</v>
       </c>
       <c r="I70" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="J70" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K70" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B71" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C71" t="n">
-        <v>4.76</v>
+        <v>4.36</v>
       </c>
       <c r="D71"/>
       <c r="E71" t="n">
-        <v>5.1</v>
+        <v>4.34</v>
       </c>
       <c r="F71" t="n">
-        <v>4.28</v>
+        <v>4.16</v>
       </c>
       <c r="G71"/>
       <c r="H71" t="n">
-        <v>4.28</v>
+        <v>4.16</v>
       </c>
       <c r="I71" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="J71" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="K71" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B72" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C72" t="n">
-        <v>4.69</v>
+        <v>4.39</v>
       </c>
       <c r="D72"/>
-      <c r="E72" t="n">
-        <v>4.48</v>
-      </c>
+      <c r="E72"/>
       <c r="F72" t="n">
-        <v>4.29</v>
+        <v>4.22</v>
       </c>
       <c r="G72"/>
       <c r="H72" t="n">
-        <v>4.29</v>
+        <v>4.22</v>
       </c>
       <c r="I72" t="s">
         <v>13</v>
@@ -3202,178 +3208,180 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B73" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C73" t="n">
-        <v>5.05</v>
+        <v>4.52</v>
       </c>
       <c r="D73"/>
       <c r="E73"/>
       <c r="F73" t="n">
-        <v>4.32</v>
+        <v>4.23</v>
       </c>
       <c r="G73"/>
       <c r="H73" t="n">
-        <v>4.32</v>
+        <v>4.23</v>
       </c>
       <c r="I73" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="J73" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="K73" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B74" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C74" t="n">
-        <v>4.07</v>
+        <v>3.06</v>
       </c>
       <c r="D74"/>
       <c r="E74"/>
       <c r="F74" t="n">
-        <v>4.32</v>
+        <v>4.24</v>
       </c>
       <c r="G74"/>
       <c r="H74" t="n">
-        <v>4.32</v>
+        <v>4.24</v>
       </c>
       <c r="I74" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="J74" t="s">
         <v>19</v>
       </c>
       <c r="K74" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B75" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C75" t="n">
-        <v>4.89</v>
+        <v>3.19</v>
       </c>
       <c r="D75"/>
-      <c r="E75"/>
+      <c r="E75" t="n">
+        <v>5.1</v>
+      </c>
       <c r="F75" t="n">
-        <v>4.34</v>
+        <v>4.28</v>
       </c>
       <c r="G75"/>
       <c r="H75" t="n">
-        <v>4.34</v>
+        <v>4.28</v>
       </c>
       <c r="I75" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="J75" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="K75" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B76" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C76" t="n">
-        <v>4.44</v>
+        <v>3.39</v>
       </c>
       <c r="D76"/>
-      <c r="E76" t="n">
-        <v>4.77</v>
-      </c>
+      <c r="E76"/>
       <c r="F76" t="n">
-        <v>4.41</v>
+        <v>4.32</v>
       </c>
       <c r="G76"/>
       <c r="H76" t="n">
-        <v>4.41</v>
+        <v>4.32</v>
       </c>
       <c r="I76" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J76" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K76" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B77" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C77" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="D77" t="n">
-        <v>4.42</v>
-      </c>
+        <v>3.13</v>
+      </c>
+      <c r="D77"/>
       <c r="E77" t="n">
-        <v>5.22</v>
+        <v>4.77</v>
       </c>
       <c r="F77" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="G77" t="n">
-        <v>5.03</v>
-      </c>
+        <v>4.41</v>
+      </c>
+      <c r="G77"/>
       <c r="H77" t="n">
-        <v>4.42</v>
+        <v>4.41</v>
       </c>
       <c r="I77" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="J77" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="K77" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B78" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C78" t="n">
-        <v>4.62</v>
+        <v>3.27</v>
       </c>
       <c r="D78" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E78"/>
-      <c r="F78"/>
-      <c r="G78"/>
+        <v>4.42</v>
+      </c>
+      <c r="E78" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="F78" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="G78" t="n">
+        <v>5.03</v>
+      </c>
       <c r="H78" t="n">
-        <v>4.5</v>
+        <v>4.42</v>
       </c>
       <c r="I78" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="J78" t="s">
         <v>19</v>
@@ -3384,80 +3392,82 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B79" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C79" t="n">
-        <v>4.98</v>
+        <v>4.4</v>
       </c>
       <c r="D79"/>
-      <c r="E79" t="n">
-        <v>4.52</v>
-      </c>
-      <c r="F79"/>
+      <c r="E79"/>
+      <c r="F79" t="n">
+        <v>4.49</v>
+      </c>
       <c r="G79"/>
       <c r="H79" t="n">
-        <v>4.52</v>
+        <v>4.49</v>
       </c>
       <c r="I79" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="J79" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="K79" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B80" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C80" t="n">
-        <v>4.16</v>
-      </c>
-      <c r="D80"/>
+        <v>4.32</v>
+      </c>
+      <c r="D80" t="n">
+        <v>4.5</v>
+      </c>
       <c r="E80"/>
-      <c r="F80" t="n">
-        <v>4.56</v>
-      </c>
+      <c r="F80"/>
       <c r="G80"/>
       <c r="H80" t="n">
-        <v>4.56</v>
+        <v>4.5</v>
       </c>
       <c r="I80" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="J80" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="K80" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B81" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C81" t="n">
-        <v>5.61</v>
+        <v>4.19</v>
       </c>
       <c r="D81"/>
-      <c r="E81"/>
+      <c r="E81" t="n">
+        <v>4.63</v>
+      </c>
       <c r="F81" t="n">
-        <v>4.57</v>
+        <v>4.52</v>
       </c>
       <c r="G81"/>
       <c r="H81" t="n">
-        <v>4.57</v>
+        <v>4.52</v>
       </c>
       <c r="I81" t="s">
         <v>13</v>
@@ -3471,22 +3481,22 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B82" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C82" t="n">
-        <v>5.34</v>
+        <v>3.94</v>
       </c>
       <c r="D82"/>
-      <c r="E82"/>
-      <c r="F82" t="n">
-        <v>4.64</v>
-      </c>
+      <c r="E82" t="n">
+        <v>4.52</v>
+      </c>
+      <c r="F82"/>
       <c r="G82"/>
       <c r="H82" t="n">
-        <v>4.64</v>
+        <v>4.52</v>
       </c>
       <c r="I82" t="s">
         <v>18</v>
@@ -3500,80 +3510,80 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B83" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C83" t="n">
-        <v>4.36</v>
-      </c>
-      <c r="D83" t="n">
-        <v>4.7</v>
-      </c>
+        <v>3.69</v>
+      </c>
+      <c r="D83"/>
       <c r="E83"/>
-      <c r="F83"/>
+      <c r="F83" t="n">
+        <v>4.57</v>
+      </c>
       <c r="G83"/>
       <c r="H83" t="n">
-        <v>4.7</v>
+        <v>4.57</v>
       </c>
       <c r="I83" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="J83" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K83" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B84" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C84" t="n">
-        <v>5.41</v>
-      </c>
-      <c r="D84"/>
+        <v>4.78</v>
+      </c>
+      <c r="D84" t="n">
+        <v>4.59</v>
+      </c>
       <c r="E84"/>
-      <c r="F84" t="n">
-        <v>4.72</v>
-      </c>
+      <c r="F84"/>
       <c r="G84"/>
       <c r="H84" t="n">
-        <v>4.72</v>
+        <v>4.59</v>
       </c>
       <c r="I84" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="J84" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="K84" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B85" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C85" t="n">
-        <v>5.65</v>
+        <v>4</v>
       </c>
       <c r="D85"/>
       <c r="E85"/>
       <c r="F85" t="n">
-        <v>4.72</v>
+        <v>4.64</v>
       </c>
       <c r="G85"/>
       <c r="H85" t="n">
-        <v>4.72</v>
+        <v>4.64</v>
       </c>
       <c r="I85" t="s">
         <v>13</v>
@@ -3587,143 +3597,141 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B86" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C86" t="n">
-        <v>5.34</v>
+        <v>4.72</v>
       </c>
       <c r="D86"/>
-      <c r="E86" t="n">
-        <v>4.74</v>
-      </c>
-      <c r="F86"/>
+      <c r="E86"/>
+      <c r="F86" t="n">
+        <v>4.71</v>
+      </c>
       <c r="G86"/>
       <c r="H86" t="n">
-        <v>4.74</v>
+        <v>4.71</v>
       </c>
       <c r="I86" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="J86" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="K86" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B87" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C87" t="n">
-        <v>4.96</v>
+        <v>5.41</v>
       </c>
       <c r="D87"/>
       <c r="E87"/>
       <c r="F87" t="n">
-        <v>4.85</v>
+        <v>4.72</v>
       </c>
       <c r="G87"/>
       <c r="H87" t="n">
-        <v>4.85</v>
+        <v>4.72</v>
       </c>
       <c r="I87" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="J87" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="K87" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B88" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C88" t="n">
-        <v>3.74</v>
+        <v>3.02</v>
       </c>
       <c r="D88"/>
       <c r="E88"/>
       <c r="F88" t="n">
-        <v>4.87</v>
+        <v>4.72</v>
       </c>
       <c r="G88"/>
       <c r="H88" t="n">
-        <v>4.87</v>
+        <v>4.72</v>
       </c>
       <c r="I88" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="J88" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K88" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B89" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C89" t="n">
-        <v>5.09</v>
+        <v>4.07</v>
       </c>
       <c r="D89"/>
       <c r="E89" t="n">
-        <v>5.01</v>
-      </c>
-      <c r="F89" t="n">
-        <v>4.9</v>
-      </c>
+        <v>4.74</v>
+      </c>
+      <c r="F89"/>
       <c r="G89"/>
       <c r="H89" t="n">
-        <v>4.9</v>
+        <v>4.74</v>
       </c>
       <c r="I89" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="J89" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="K89" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B90" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C90" t="n">
         <v>3.66</v>
       </c>
       <c r="D90" t="n">
-        <v>4.94</v>
+        <v>4.76</v>
       </c>
       <c r="E90"/>
       <c r="F90"/>
       <c r="G90"/>
       <c r="H90" t="n">
-        <v>4.94</v>
+        <v>4.76</v>
       </c>
       <c r="I90" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="J90" t="s">
         <v>14</v>
@@ -3734,115 +3742,115 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B91" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C91" t="n">
-        <v>5.73</v>
-      </c>
-      <c r="D91" t="n">
-        <v>5.08</v>
-      </c>
+        <v>4.45</v>
+      </c>
+      <c r="D91"/>
       <c r="E91"/>
-      <c r="F91"/>
+      <c r="F91" t="n">
+        <v>4.86</v>
+      </c>
       <c r="G91"/>
       <c r="H91" t="n">
-        <v>5.08</v>
+        <v>4.86</v>
       </c>
       <c r="I91" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="J91" t="s">
         <v>19</v>
       </c>
       <c r="K91" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B92" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C92" t="n">
-        <v>5.52</v>
-      </c>
-      <c r="D92"/>
+        <v>5.22</v>
+      </c>
+      <c r="D92" t="n">
+        <v>4.88</v>
+      </c>
       <c r="E92"/>
       <c r="F92"/>
-      <c r="G92" t="n">
-        <v>5.12</v>
-      </c>
+      <c r="G92"/>
       <c r="H92" t="n">
-        <v>5.12</v>
+        <v>4.88</v>
       </c>
       <c r="I92" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="J92" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="K92" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B93" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C93" t="n">
-        <v>5.97</v>
-      </c>
-      <c r="D93" t="n">
-        <v>5.17</v>
-      </c>
+        <v>3.82</v>
+      </c>
+      <c r="D93"/>
       <c r="E93"/>
       <c r="F93"/>
-      <c r="G93"/>
+      <c r="G93" t="n">
+        <v>5.12</v>
+      </c>
       <c r="H93" t="n">
-        <v>5.17</v>
+        <v>5.12</v>
       </c>
       <c r="I93" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J93" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="K93" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B94" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C94" t="n">
-        <v>6.34</v>
+        <v>5.07</v>
       </c>
       <c r="D94" t="n">
-        <v>5.45</v>
+        <v>5.17</v>
       </c>
       <c r="E94"/>
       <c r="F94"/>
       <c r="G94"/>
       <c r="H94" t="n">
-        <v>5.45</v>
+        <v>5.17</v>
       </c>
       <c r="I94" t="s">
         <v>24</v>
       </c>
       <c r="J94" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K94" t="s">
         <v>25</v>
@@ -3850,10 +3858,10 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B95" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C95" t="n">
         <v>5.84</v>
@@ -3861,11 +3869,11 @@
       <c r="D95"/>
       <c r="E95"/>
       <c r="F95" t="n">
-        <v>5.55</v>
+        <v>5.27</v>
       </c>
       <c r="G95"/>
       <c r="H95" t="n">
-        <v>5.55</v>
+        <v>5.27</v>
       </c>
       <c r="I95" t="s">
         <v>13</v>
@@ -3879,119 +3887,179 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B96" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C96" t="n">
-        <v>6.29</v>
-      </c>
-      <c r="D96"/>
+        <v>5.43</v>
+      </c>
+      <c r="D96" t="n">
+        <v>5.45</v>
+      </c>
       <c r="E96"/>
       <c r="F96"/>
-      <c r="G96" t="n">
-        <v>6.26</v>
-      </c>
+      <c r="G96"/>
       <c r="H96" t="n">
-        <v>6.26</v>
+        <v>5.45</v>
       </c>
       <c r="I96" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="J96" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="K96" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B97" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C97" t="n">
-        <v>7.23</v>
+        <v>4.84</v>
       </c>
       <c r="D97"/>
       <c r="E97" t="n">
-        <v>6.74</v>
+        <v>6.29</v>
       </c>
       <c r="F97" t="n">
-        <v>6.62</v>
+        <v>5.54</v>
       </c>
       <c r="G97"/>
       <c r="H97" t="n">
-        <v>6.62</v>
+        <v>5.54</v>
       </c>
       <c r="I97" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="J97" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="K97" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B98" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C98" t="n">
-        <v>8.54</v>
-      </c>
-      <c r="D98" t="n">
-        <v>7.15</v>
-      </c>
+        <v>5.62</v>
+      </c>
+      <c r="D98"/>
       <c r="E98"/>
       <c r="F98"/>
-      <c r="G98"/>
+      <c r="G98" t="n">
+        <v>6.26</v>
+      </c>
       <c r="H98" t="n">
-        <v>7.15</v>
+        <v>6.26</v>
       </c>
       <c r="I98" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="J98" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="K98" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B99" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C99" t="n">
-        <v>8.04</v>
-      </c>
-      <c r="D99" t="n">
-        <v>7.27</v>
-      </c>
-      <c r="E99"/>
-      <c r="F99"/>
+        <v>7.23</v>
+      </c>
+      <c r="D99"/>
+      <c r="E99" t="n">
+        <v>6.74</v>
+      </c>
+      <c r="F99" t="n">
+        <v>6.62</v>
+      </c>
       <c r="G99"/>
       <c r="H99" t="n">
+        <v>6.62</v>
+      </c>
+      <c r="I99" t="s">
+        <v>13</v>
+      </c>
+      <c r="J99" t="s">
+        <v>14</v>
+      </c>
+      <c r="K99" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>215</v>
+      </c>
+      <c r="B100" t="s">
+        <v>216</v>
+      </c>
+      <c r="C100" t="n">
+        <v>6.65</v>
+      </c>
+      <c r="D100" t="n">
+        <v>7.15</v>
+      </c>
+      <c r="E100"/>
+      <c r="F100"/>
+      <c r="G100"/>
+      <c r="H100" t="n">
+        <v>7.15</v>
+      </c>
+      <c r="I100" t="s">
+        <v>24</v>
+      </c>
+      <c r="J100" t="s">
+        <v>14</v>
+      </c>
+      <c r="K100" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>217</v>
+      </c>
+      <c r="B101" t="s">
+        <v>218</v>
+      </c>
+      <c r="C101" t="n">
+        <v>6.99</v>
+      </c>
+      <c r="D101" t="n">
         <v>7.27</v>
       </c>
-      <c r="I99" t="s">
+      <c r="E101"/>
+      <c r="F101"/>
+      <c r="G101"/>
+      <c r="H101" t="n">
+        <v>7.27</v>
+      </c>
+      <c r="I101" t="s">
         <v>24</v>
       </c>
-      <c r="J99" t="s">
-        <v>19</v>
-      </c>
-      <c r="K99" t="s">
+      <c r="J101" t="s">
+        <v>14</v>
+      </c>
+      <c r="K101" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reran vignette after compiling feature/fullterm_pregnancy
</commit_message>
<xml_diff>
--- a/tables/plasma_and_tissueBERs.xlsx
+++ b/tables/plasma_and_tissueBERs.xlsx
@@ -1043,7 +1043,7 @@
         <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.61</v>
+        <v>-2.74</v>
       </c>
       <c r="D2"/>
       <c r="E2"/>
@@ -1072,7 +1072,7 @@
         <v>17</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6</v>
+        <v>4.69</v>
       </c>
       <c r="D3" t="n">
         <v>-1.21</v>
@@ -1105,7 +1105,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6</v>
+        <v>4.69</v>
       </c>
       <c r="D4" t="n">
         <v>-1.21</v>
@@ -1138,7 +1138,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.36</v>
+        <v>-0.28</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="n">
@@ -1169,7 +1169,7 @@
         <v>23</v>
       </c>
       <c r="C6" t="n">
-        <v>0.07</v>
+        <v>0.11</v>
       </c>
       <c r="D6" t="n">
         <v>-0.66</v>
@@ -1202,7 +1202,7 @@
         <v>27</v>
       </c>
       <c r="C7" t="n">
-        <v>2.76</v>
+        <v>5.73</v>
       </c>
       <c r="D7"/>
       <c r="E7"/>
@@ -1231,7 +1231,7 @@
         <v>29</v>
       </c>
       <c r="C8" t="n">
-        <v>0.09</v>
+        <v>1.17</v>
       </c>
       <c r="D8" t="n">
         <v>0.27</v>
@@ -1264,7 +1264,7 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>0.28</v>
+        <v>0.38</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="n">
@@ -1328,7 +1328,7 @@
         <v>37</v>
       </c>
       <c r="C11" t="n">
-        <v>0.98</v>
+        <v>2.14</v>
       </c>
       <c r="D11"/>
       <c r="E11"/>
@@ -1359,7 +1359,7 @@
         <v>39</v>
       </c>
       <c r="C12" t="n">
-        <v>0.31</v>
+        <v>1.38</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="C13" t="n">
-        <v>2.78</v>
+        <v>1.1</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="n">
@@ -1419,7 +1419,7 @@
         <v>43</v>
       </c>
       <c r="C14" t="n">
-        <v>1.03</v>
+        <v>2.46</v>
       </c>
       <c r="D14" t="n">
         <v>2.93</v>
@@ -1452,7 +1452,7 @@
         <v>45</v>
       </c>
       <c r="C15" t="n">
-        <v>1.6</v>
+        <v>1.9</v>
       </c>
       <c r="D15" t="n">
         <v>1.56</v>
@@ -1485,7 +1485,7 @@
         <v>47</v>
       </c>
       <c r="C16" t="n">
-        <v>3.3</v>
+        <v>0.49</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="n">
@@ -1516,7 +1516,7 @@
         <v>49</v>
       </c>
       <c r="C17" t="n">
-        <v>3.42</v>
+        <v>2.46</v>
       </c>
       <c r="D17" t="n">
         <v>1.65</v>
@@ -1547,7 +1547,7 @@
         <v>49</v>
       </c>
       <c r="C18" t="n">
-        <v>3.42</v>
+        <v>2.46</v>
       </c>
       <c r="D18" t="n">
         <v>1.65</v>
@@ -1578,7 +1578,7 @@
         <v>52</v>
       </c>
       <c r="C19" t="n">
-        <v>1.39</v>
+        <v>2.22</v>
       </c>
       <c r="D19"/>
       <c r="E19" t="n">
@@ -1609,7 +1609,7 @@
         <v>54</v>
       </c>
       <c r="C20" t="n">
-        <v>1.33</v>
+        <v>2.17</v>
       </c>
       <c r="D20" t="n">
         <v>1.8</v>
@@ -1640,7 +1640,7 @@
         <v>56</v>
       </c>
       <c r="C21" t="n">
-        <v>2.52</v>
+        <v>1.57</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="n">
@@ -1671,7 +1671,7 @@
         <v>58</v>
       </c>
       <c r="C22" t="n">
-        <v>1.5</v>
+        <v>2.49</v>
       </c>
       <c r="D22" t="n">
         <v>1.98</v>
@@ -1700,7 +1700,7 @@
         <v>60</v>
       </c>
       <c r="C23" t="n">
-        <v>0.85</v>
+        <v>2.54</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="n">
@@ -1731,7 +1731,7 @@
         <v>64</v>
       </c>
       <c r="C24" t="n">
-        <v>2.82</v>
+        <v>2.11</v>
       </c>
       <c r="D24"/>
       <c r="E24" t="n">
@@ -1762,7 +1762,7 @@
         <v>66</v>
       </c>
       <c r="C25" t="n">
-        <v>2.23</v>
+        <v>2.76</v>
       </c>
       <c r="D25" t="n">
         <v>2.05</v>
@@ -1791,7 +1791,7 @@
         <v>68</v>
       </c>
       <c r="C26" t="n">
-        <v>1.5</v>
+        <v>3.09</v>
       </c>
       <c r="D26"/>
       <c r="E26" t="n">
@@ -1822,7 +1822,7 @@
         <v>70</v>
       </c>
       <c r="C27" t="n">
-        <v>3.45</v>
+        <v>2.29</v>
       </c>
       <c r="D27" t="n">
         <v>2.24</v>
@@ -1853,7 +1853,7 @@
         <v>72</v>
       </c>
       <c r="C28" t="n">
-        <v>3.5</v>
+        <v>3.18</v>
       </c>
       <c r="D28" t="n">
         <v>2.26</v>
@@ -1882,7 +1882,7 @@
         <v>74</v>
       </c>
       <c r="C29" t="n">
-        <v>2.36</v>
+        <v>3.1</v>
       </c>
       <c r="D29" t="n">
         <v>2.52</v>
@@ -1911,7 +1911,7 @@
         <v>76</v>
       </c>
       <c r="C30" t="n">
-        <v>1.99</v>
+        <v>2.92</v>
       </c>
       <c r="D30" t="n">
         <v>2.52</v>
@@ -1944,7 +1944,7 @@
         <v>78</v>
       </c>
       <c r="C31" t="n">
-        <v>2.05</v>
+        <v>3.07</v>
       </c>
       <c r="D31"/>
       <c r="E31"/>
@@ -1973,7 +1973,7 @@
         <v>80</v>
       </c>
       <c r="C32" t="n">
-        <v>2.65</v>
+        <v>3.14</v>
       </c>
       <c r="D32"/>
       <c r="E32"/>
@@ -2002,7 +2002,7 @@
         <v>82</v>
       </c>
       <c r="C33" t="n">
-        <v>2.73</v>
+        <v>3.06</v>
       </c>
       <c r="D33"/>
       <c r="E33"/>
@@ -2031,7 +2031,7 @@
         <v>84</v>
       </c>
       <c r="C34" t="n">
-        <v>2.27</v>
+        <v>3.08</v>
       </c>
       <c r="D34" t="n">
         <v>2.59</v>
@@ -2093,7 +2093,7 @@
         <v>88</v>
       </c>
       <c r="C36" t="n">
-        <v>2.43</v>
+        <v>2.95</v>
       </c>
       <c r="D36"/>
       <c r="E36"/>
@@ -2122,7 +2122,7 @@
         <v>90</v>
       </c>
       <c r="C37" t="n">
-        <v>2.18</v>
+        <v>3.26</v>
       </c>
       <c r="D37" t="n">
         <v>2.66</v>
@@ -2155,7 +2155,7 @@
         <v>92</v>
       </c>
       <c r="C38" t="n">
-        <v>4.05</v>
+        <v>2.38</v>
       </c>
       <c r="D38"/>
       <c r="E38"/>
@@ -2184,7 +2184,7 @@
         <v>94</v>
       </c>
       <c r="C39" t="n">
-        <v>2.64</v>
+        <v>3.03</v>
       </c>
       <c r="D39"/>
       <c r="E39"/>
@@ -2213,7 +2213,7 @@
         <v>96</v>
       </c>
       <c r="C40" t="n">
-        <v>3.15</v>
+        <v>3.47</v>
       </c>
       <c r="D40"/>
       <c r="E40"/>
@@ -2244,7 +2244,7 @@
         <v>98</v>
       </c>
       <c r="C41" t="n">
-        <v>1.75</v>
+        <v>3.63</v>
       </c>
       <c r="D41"/>
       <c r="E41" t="n">
@@ -2275,7 +2275,7 @@
         <v>100</v>
       </c>
       <c r="C42" t="n">
-        <v>4.33</v>
+        <v>2.25</v>
       </c>
       <c r="D42" t="n">
         <v>3.41</v>
@@ -2310,7 +2310,7 @@
         <v>102</v>
       </c>
       <c r="C43" t="n">
-        <v>2.73</v>
+        <v>3.67</v>
       </c>
       <c r="D43" t="n">
         <v>2.89</v>
@@ -2339,7 +2339,7 @@
         <v>104</v>
       </c>
       <c r="C44" t="n">
-        <v>1.91</v>
+        <v>2.44</v>
       </c>
       <c r="D44" t="n">
         <v>3.19</v>
@@ -2372,7 +2372,7 @@
         <v>106</v>
       </c>
       <c r="C45" t="n">
-        <v>2.77</v>
+        <v>3.17</v>
       </c>
       <c r="D45"/>
       <c r="E45" t="n">
@@ -2403,7 +2403,7 @@
         <v>108</v>
       </c>
       <c r="C46" t="n">
-        <v>2.57</v>
+        <v>3.84</v>
       </c>
       <c r="D46" t="n">
         <v>2.97</v>
@@ -2434,7 +2434,7 @@
         <v>110</v>
       </c>
       <c r="C47" t="n">
-        <v>3.02</v>
+        <v>3.93</v>
       </c>
       <c r="D47" t="n">
         <v>2.97</v>
@@ -2463,7 +2463,7 @@
         <v>112</v>
       </c>
       <c r="C48" t="n">
-        <v>3.71</v>
+        <v>4.2</v>
       </c>
       <c r="D48"/>
       <c r="E48"/>
@@ -2492,7 +2492,7 @@
         <v>114</v>
       </c>
       <c r="C49" t="n">
-        <v>2.15</v>
+        <v>3.17</v>
       </c>
       <c r="D49"/>
       <c r="E49" t="n">
@@ -2525,7 +2525,7 @@
         <v>116</v>
       </c>
       <c r="C50" t="n">
-        <v>2.26</v>
+        <v>3.32</v>
       </c>
       <c r="D50"/>
       <c r="E50"/>
@@ -2554,7 +2554,7 @@
         <v>118</v>
       </c>
       <c r="C51" t="n">
-        <v>2.54</v>
+        <v>3.64</v>
       </c>
       <c r="D51"/>
       <c r="E51" t="n">
@@ -2585,7 +2585,7 @@
         <v>120</v>
       </c>
       <c r="C52" t="n">
-        <v>1.56</v>
+        <v>3.38</v>
       </c>
       <c r="D52"/>
       <c r="E52"/>
@@ -2614,7 +2614,7 @@
         <v>122</v>
       </c>
       <c r="C53" t="n">
-        <v>2.55</v>
+        <v>3.85</v>
       </c>
       <c r="D53" t="n">
         <v>3.42</v>
@@ -2647,7 +2647,7 @@
         <v>124</v>
       </c>
       <c r="C54" t="n">
-        <v>3.2</v>
+        <v>3.42</v>
       </c>
       <c r="D54"/>
       <c r="E54" t="n">
@@ -2678,7 +2678,7 @@
         <v>126</v>
       </c>
       <c r="C55" t="n">
-        <v>3.56</v>
+        <v>3.93</v>
       </c>
       <c r="D55" t="n">
         <v>3.51</v>
@@ -2707,7 +2707,7 @@
         <v>128</v>
       </c>
       <c r="C56" t="n">
-        <v>3.61</v>
+        <v>2.25</v>
       </c>
       <c r="D56" t="n">
         <v>3.75</v>
@@ -2740,7 +2740,7 @@
         <v>130</v>
       </c>
       <c r="C57" t="n">
-        <v>4.27</v>
+        <v>4.33</v>
       </c>
       <c r="D57"/>
       <c r="E57"/>
@@ -2769,7 +2769,7 @@
         <v>132</v>
       </c>
       <c r="C58" t="n">
-        <v>3.36</v>
+        <v>4.47</v>
       </c>
       <c r="D58" t="n">
         <v>3.54</v>
@@ -2798,7 +2798,7 @@
         <v>134</v>
       </c>
       <c r="C59" t="n">
-        <v>3.04</v>
+        <v>3.5</v>
       </c>
       <c r="D59"/>
       <c r="E59" t="n">
@@ -2829,7 +2829,7 @@
         <v>136</v>
       </c>
       <c r="C60" t="n">
-        <v>5.2</v>
+        <v>3.58</v>
       </c>
       <c r="D60"/>
       <c r="E60"/>
@@ -2858,7 +2858,7 @@
         <v>138</v>
       </c>
       <c r="C61" t="n">
-        <v>2.62</v>
+        <v>5.09</v>
       </c>
       <c r="D61" t="n">
         <v>3.66</v>
@@ -2887,7 +2887,7 @@
         <v>140</v>
       </c>
       <c r="C62" t="n">
-        <v>3.66</v>
+        <v>4.68</v>
       </c>
       <c r="D62" t="n">
         <v>3.66</v>
@@ -2920,7 +2920,7 @@
         <v>142</v>
       </c>
       <c r="C63" t="n">
-        <v>2.86</v>
+        <v>3.59</v>
       </c>
       <c r="D63"/>
       <c r="E63" t="n">
@@ -2951,7 +2951,7 @@
         <v>144</v>
       </c>
       <c r="C64" t="n">
-        <v>3.73</v>
+        <v>3.96</v>
       </c>
       <c r="D64"/>
       <c r="E64"/>
@@ -2980,7 +2980,7 @@
         <v>146</v>
       </c>
       <c r="C65" t="n">
-        <v>3.31</v>
+        <v>4.23</v>
       </c>
       <c r="D65" t="n">
         <v>3.87</v>
@@ -3009,7 +3009,7 @@
         <v>148</v>
       </c>
       <c r="C66" t="n">
-        <v>3.13</v>
+        <v>5.29</v>
       </c>
       <c r="D66" t="n">
         <v>3.97</v>
@@ -3038,7 +3038,7 @@
         <v>150</v>
       </c>
       <c r="C67" t="n">
-        <v>3.5</v>
+        <v>4.33</v>
       </c>
       <c r="D67"/>
       <c r="E67"/>
@@ -3067,7 +3067,7 @@
         <v>152</v>
       </c>
       <c r="C68" t="n">
-        <v>3.74</v>
+        <v>4.44</v>
       </c>
       <c r="D68"/>
       <c r="E68" t="n">
@@ -3096,7 +3096,7 @@
         <v>154</v>
       </c>
       <c r="C69" t="n">
-        <v>3.31</v>
+        <v>4.06</v>
       </c>
       <c r="D69"/>
       <c r="E69" t="n">
@@ -3125,7 +3125,7 @@
         <v>156</v>
       </c>
       <c r="C70" t="n">
-        <v>5.98</v>
+        <v>3.31</v>
       </c>
       <c r="D70" t="n">
         <v>4.11</v>
@@ -3154,7 +3154,7 @@
         <v>158</v>
       </c>
       <c r="C71" t="n">
-        <v>4.36</v>
+        <v>4.69</v>
       </c>
       <c r="D71"/>
       <c r="E71" t="n">
@@ -3185,7 +3185,7 @@
         <v>160</v>
       </c>
       <c r="C72" t="n">
-        <v>4.39</v>
+        <v>4.07</v>
       </c>
       <c r="D72"/>
       <c r="E72"/>
@@ -3214,7 +3214,7 @@
         <v>162</v>
       </c>
       <c r="C73" t="n">
-        <v>4.52</v>
+        <v>4.89</v>
       </c>
       <c r="D73"/>
       <c r="E73"/>
@@ -3243,7 +3243,7 @@
         <v>164</v>
       </c>
       <c r="C74" t="n">
-        <v>3.06</v>
+        <v>5.05</v>
       </c>
       <c r="D74"/>
       <c r="E74"/>
@@ -3272,7 +3272,7 @@
         <v>166</v>
       </c>
       <c r="C75" t="n">
-        <v>3.19</v>
+        <v>4.76</v>
       </c>
       <c r="D75"/>
       <c r="E75" t="n">
@@ -3303,7 +3303,7 @@
         <v>168</v>
       </c>
       <c r="C76" t="n">
-        <v>3.39</v>
+        <v>5.05</v>
       </c>
       <c r="D76"/>
       <c r="E76"/>
@@ -3332,7 +3332,7 @@
         <v>170</v>
       </c>
       <c r="C77" t="n">
-        <v>3.13</v>
+        <v>4.44</v>
       </c>
       <c r="D77"/>
       <c r="E77" t="n">
@@ -3363,7 +3363,7 @@
         <v>172</v>
       </c>
       <c r="C78" t="n">
-        <v>3.27</v>
+        <v>4.8</v>
       </c>
       <c r="D78" t="n">
         <v>4.42</v>
@@ -3398,7 +3398,7 @@
         <v>174</v>
       </c>
       <c r="C79" t="n">
-        <v>4.4</v>
+        <v>4.16</v>
       </c>
       <c r="D79"/>
       <c r="E79"/>
@@ -3427,7 +3427,7 @@
         <v>176</v>
       </c>
       <c r="C80" t="n">
-        <v>4.32</v>
+        <v>4.62</v>
       </c>
       <c r="D80" t="n">
         <v>4.5</v>
@@ -3456,7 +3456,7 @@
         <v>178</v>
       </c>
       <c r="C81" t="n">
-        <v>4.19</v>
+        <v>5.09</v>
       </c>
       <c r="D81"/>
       <c r="E81" t="n">
@@ -3487,7 +3487,7 @@
         <v>180</v>
       </c>
       <c r="C82" t="n">
-        <v>3.94</v>
+        <v>4.98</v>
       </c>
       <c r="D82"/>
       <c r="E82" t="n">
@@ -3516,7 +3516,7 @@
         <v>182</v>
       </c>
       <c r="C83" t="n">
-        <v>3.69</v>
+        <v>5.61</v>
       </c>
       <c r="D83"/>
       <c r="E83"/>
@@ -3545,7 +3545,7 @@
         <v>184</v>
       </c>
       <c r="C84" t="n">
-        <v>4.78</v>
+        <v>4.36</v>
       </c>
       <c r="D84" t="n">
         <v>4.59</v>
@@ -3574,7 +3574,7 @@
         <v>186</v>
       </c>
       <c r="C85" t="n">
-        <v>4</v>
+        <v>5.34</v>
       </c>
       <c r="D85"/>
       <c r="E85"/>
@@ -3603,7 +3603,7 @@
         <v>188</v>
       </c>
       <c r="C86" t="n">
-        <v>4.72</v>
+        <v>4.96</v>
       </c>
       <c r="D86"/>
       <c r="E86"/>
@@ -3661,7 +3661,7 @@
         <v>192</v>
       </c>
       <c r="C88" t="n">
-        <v>3.02</v>
+        <v>5.65</v>
       </c>
       <c r="D88"/>
       <c r="E88"/>
@@ -3690,7 +3690,7 @@
         <v>194</v>
       </c>
       <c r="C89" t="n">
-        <v>4.07</v>
+        <v>5.34</v>
       </c>
       <c r="D89"/>
       <c r="E89" t="n">
@@ -3748,7 +3748,7 @@
         <v>198</v>
       </c>
       <c r="C91" t="n">
-        <v>4.45</v>
+        <v>3.74</v>
       </c>
       <c r="D91"/>
       <c r="E91"/>
@@ -3777,7 +3777,7 @@
         <v>200</v>
       </c>
       <c r="C92" t="n">
-        <v>5.22</v>
+        <v>5.73</v>
       </c>
       <c r="D92" t="n">
         <v>4.88</v>
@@ -3806,7 +3806,7 @@
         <v>202</v>
       </c>
       <c r="C93" t="n">
-        <v>3.82</v>
+        <v>5.52</v>
       </c>
       <c r="D93"/>
       <c r="E93"/>
@@ -3835,7 +3835,7 @@
         <v>204</v>
       </c>
       <c r="C94" t="n">
-        <v>5.07</v>
+        <v>5.97</v>
       </c>
       <c r="D94" t="n">
         <v>5.17</v>
@@ -3893,7 +3893,7 @@
         <v>208</v>
       </c>
       <c r="C96" t="n">
-        <v>5.43</v>
+        <v>6.34</v>
       </c>
       <c r="D96" t="n">
         <v>5.45</v>
@@ -3922,7 +3922,7 @@
         <v>210</v>
       </c>
       <c r="C97" t="n">
-        <v>4.84</v>
+        <v>6.07</v>
       </c>
       <c r="D97"/>
       <c r="E97" t="n">
@@ -3953,7 +3953,7 @@
         <v>212</v>
       </c>
       <c r="C98" t="n">
-        <v>5.62</v>
+        <v>6.29</v>
       </c>
       <c r="D98"/>
       <c r="E98"/>
@@ -4013,7 +4013,7 @@
         <v>216</v>
       </c>
       <c r="C100" t="n">
-        <v>6.65</v>
+        <v>8.54</v>
       </c>
       <c r="D100" t="n">
         <v>7.15</v>
@@ -4042,7 +4042,7 @@
         <v>218</v>
       </c>
       <c r="C101" t="n">
-        <v>6.99</v>
+        <v>8.04</v>
       </c>
       <c r="D101" t="n">
         <v>7.27</v>

</xml_diff>

<commit_message>
pushed updates to figures after merging into dev
</commit_message>
<xml_diff>
--- a/tables/plasma_and_tissueBERs.xlsx
+++ b/tables/plasma_and_tissueBERs.xlsx
@@ -1043,7 +1043,7 @@
         <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>-2.74</v>
+        <v>-2.5</v>
       </c>
       <c r="D2"/>
       <c r="E2"/>
@@ -1072,7 +1072,7 @@
         <v>17</v>
       </c>
       <c r="C3" t="n">
-        <v>4.69</v>
+        <v>2.78</v>
       </c>
       <c r="D3" t="n">
         <v>-1.21</v>
@@ -1105,7 +1105,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="n">
-        <v>4.69</v>
+        <v>2.78</v>
       </c>
       <c r="D4" t="n">
         <v>-1.21</v>
@@ -1138,7 +1138,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.28</v>
+        <v>-0.06</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="n">
@@ -1169,7 +1169,7 @@
         <v>23</v>
       </c>
       <c r="C6" t="n">
-        <v>0.11</v>
+        <v>0.34</v>
       </c>
       <c r="D6" t="n">
         <v>-0.66</v>
@@ -1202,7 +1202,7 @@
         <v>27</v>
       </c>
       <c r="C7" t="n">
-        <v>5.73</v>
+        <v>3.7</v>
       </c>
       <c r="D7"/>
       <c r="E7"/>
@@ -1231,7 +1231,7 @@
         <v>29</v>
       </c>
       <c r="C8" t="n">
-        <v>1.17</v>
+        <v>1.28</v>
       </c>
       <c r="D8" t="n">
         <v>0.27</v>
@@ -1264,7 +1264,7 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>0.38</v>
+        <v>0.43</v>
       </c>
       <c r="D9"/>
       <c r="E9" t="n">
@@ -1295,7 +1295,7 @@
         <v>35</v>
       </c>
       <c r="C10" t="n">
-        <v>0.32</v>
+        <v>0.45</v>
       </c>
       <c r="D10" t="n">
         <v>0.76</v>
@@ -1328,7 +1328,7 @@
         <v>37</v>
       </c>
       <c r="C11" t="n">
-        <v>2.14</v>
+        <v>2.22</v>
       </c>
       <c r="D11"/>
       <c r="E11"/>
@@ -1359,7 +1359,7 @@
         <v>39</v>
       </c>
       <c r="C12" t="n">
-        <v>1.38</v>
+        <v>1.35</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
@@ -1388,7 +1388,7 @@
         <v>41</v>
       </c>
       <c r="C13" t="n">
-        <v>1.1</v>
+        <v>1.23</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="n">
@@ -1419,7 +1419,7 @@
         <v>43</v>
       </c>
       <c r="C14" t="n">
-        <v>2.46</v>
+        <v>2.77</v>
       </c>
       <c r="D14" t="n">
         <v>2.93</v>
@@ -1452,7 +1452,7 @@
         <v>45</v>
       </c>
       <c r="C15" t="n">
-        <v>1.9</v>
+        <v>2.03</v>
       </c>
       <c r="D15" t="n">
         <v>1.56</v>
@@ -1485,7 +1485,7 @@
         <v>47</v>
       </c>
       <c r="C16" t="n">
-        <v>0.49</v>
+        <v>0.62</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="n">
@@ -1516,7 +1516,7 @@
         <v>49</v>
       </c>
       <c r="C17" t="n">
-        <v>2.46</v>
+        <v>2.69</v>
       </c>
       <c r="D17" t="n">
         <v>1.65</v>
@@ -1547,7 +1547,7 @@
         <v>49</v>
       </c>
       <c r="C18" t="n">
-        <v>2.46</v>
+        <v>2.69</v>
       </c>
       <c r="D18" t="n">
         <v>1.65</v>
@@ -1578,7 +1578,7 @@
         <v>52</v>
       </c>
       <c r="C19" t="n">
-        <v>2.22</v>
+        <v>2.54</v>
       </c>
       <c r="D19"/>
       <c r="E19" t="n">
@@ -1609,7 +1609,7 @@
         <v>54</v>
       </c>
       <c r="C20" t="n">
-        <v>2.17</v>
+        <v>2.31</v>
       </c>
       <c r="D20" t="n">
         <v>1.8</v>
@@ -1640,7 +1640,7 @@
         <v>56</v>
       </c>
       <c r="C21" t="n">
-        <v>1.57</v>
+        <v>1.58</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="n">
@@ -1671,7 +1671,7 @@
         <v>58</v>
       </c>
       <c r="C22" t="n">
-        <v>2.49</v>
+        <v>2.61</v>
       </c>
       <c r="D22" t="n">
         <v>1.98</v>
@@ -1700,7 +1700,7 @@
         <v>60</v>
       </c>
       <c r="C23" t="n">
-        <v>2.54</v>
+        <v>2.72</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="n">
@@ -1731,7 +1731,7 @@
         <v>64</v>
       </c>
       <c r="C24" t="n">
-        <v>2.11</v>
+        <v>2.12</v>
       </c>
       <c r="D24"/>
       <c r="E24" t="n">
@@ -1762,7 +1762,7 @@
         <v>66</v>
       </c>
       <c r="C25" t="n">
-        <v>2.76</v>
+        <v>2.89</v>
       </c>
       <c r="D25" t="n">
         <v>2.05</v>
@@ -1791,7 +1791,7 @@
         <v>68</v>
       </c>
       <c r="C26" t="n">
-        <v>3.09</v>
+        <v>3.51</v>
       </c>
       <c r="D26"/>
       <c r="E26" t="n">
@@ -1822,7 +1822,7 @@
         <v>70</v>
       </c>
       <c r="C27" t="n">
-        <v>2.29</v>
+        <v>2.42</v>
       </c>
       <c r="D27" t="n">
         <v>2.24</v>
@@ -1853,7 +1853,7 @@
         <v>72</v>
       </c>
       <c r="C28" t="n">
-        <v>3.18</v>
+        <v>3.29</v>
       </c>
       <c r="D28" t="n">
         <v>2.26</v>
@@ -1882,7 +1882,7 @@
         <v>74</v>
       </c>
       <c r="C29" t="n">
-        <v>3.1</v>
+        <v>3.21</v>
       </c>
       <c r="D29" t="n">
         <v>2.52</v>
@@ -1911,7 +1911,7 @@
         <v>76</v>
       </c>
       <c r="C30" t="n">
-        <v>2.92</v>
+        <v>3.06</v>
       </c>
       <c r="D30" t="n">
         <v>2.52</v>
@@ -1944,7 +1944,7 @@
         <v>78</v>
       </c>
       <c r="C31" t="n">
-        <v>3.07</v>
+        <v>3.44</v>
       </c>
       <c r="D31"/>
       <c r="E31"/>
@@ -1973,7 +1973,7 @@
         <v>80</v>
       </c>
       <c r="C32" t="n">
-        <v>3.14</v>
+        <v>3.27</v>
       </c>
       <c r="D32"/>
       <c r="E32"/>
@@ -2002,7 +2002,7 @@
         <v>82</v>
       </c>
       <c r="C33" t="n">
-        <v>3.06</v>
+        <v>3.28</v>
       </c>
       <c r="D33"/>
       <c r="E33"/>
@@ -2031,7 +2031,7 @@
         <v>84</v>
       </c>
       <c r="C34" t="n">
-        <v>3.08</v>
+        <v>3.22</v>
       </c>
       <c r="D34" t="n">
         <v>2.59</v>
@@ -2062,7 +2062,7 @@
         <v>86</v>
       </c>
       <c r="C35" t="n">
-        <v>2.96</v>
+        <v>3.09</v>
       </c>
       <c r="D35"/>
       <c r="E35" t="n">
@@ -2093,7 +2093,7 @@
         <v>88</v>
       </c>
       <c r="C36" t="n">
-        <v>2.95</v>
+        <v>3.02</v>
       </c>
       <c r="D36"/>
       <c r="E36"/>
@@ -2122,7 +2122,7 @@
         <v>90</v>
       </c>
       <c r="C37" t="n">
-        <v>3.26</v>
+        <v>3.39</v>
       </c>
       <c r="D37" t="n">
         <v>2.66</v>
@@ -2155,7 +2155,7 @@
         <v>92</v>
       </c>
       <c r="C38" t="n">
-        <v>2.38</v>
+        <v>2.52</v>
       </c>
       <c r="D38"/>
       <c r="E38"/>
@@ -2184,7 +2184,7 @@
         <v>94</v>
       </c>
       <c r="C39" t="n">
-        <v>3.03</v>
+        <v>3.16</v>
       </c>
       <c r="D39"/>
       <c r="E39"/>
@@ -2213,7 +2213,7 @@
         <v>96</v>
       </c>
       <c r="C40" t="n">
-        <v>3.47</v>
+        <v>3.61</v>
       </c>
       <c r="D40"/>
       <c r="E40"/>
@@ -2244,7 +2244,7 @@
         <v>98</v>
       </c>
       <c r="C41" t="n">
-        <v>3.63</v>
+        <v>3.83</v>
       </c>
       <c r="D41"/>
       <c r="E41" t="n">
@@ -2275,7 +2275,7 @@
         <v>100</v>
       </c>
       <c r="C42" t="n">
-        <v>2.25</v>
+        <v>2.39</v>
       </c>
       <c r="D42" t="n">
         <v>3.41</v>
@@ -2310,7 +2310,7 @@
         <v>102</v>
       </c>
       <c r="C43" t="n">
-        <v>3.67</v>
+        <v>3.8</v>
       </c>
       <c r="D43" t="n">
         <v>2.89</v>
@@ -2339,7 +2339,7 @@
         <v>104</v>
       </c>
       <c r="C44" t="n">
-        <v>2.44</v>
+        <v>2.56</v>
       </c>
       <c r="D44" t="n">
         <v>3.19</v>
@@ -2372,7 +2372,7 @@
         <v>106</v>
       </c>
       <c r="C45" t="n">
-        <v>3.17</v>
+        <v>3.29</v>
       </c>
       <c r="D45"/>
       <c r="E45" t="n">
@@ -2403,7 +2403,7 @@
         <v>108</v>
       </c>
       <c r="C46" t="n">
-        <v>3.84</v>
+        <v>3.96</v>
       </c>
       <c r="D46" t="n">
         <v>2.97</v>
@@ -2434,7 +2434,7 @@
         <v>110</v>
       </c>
       <c r="C47" t="n">
-        <v>3.93</v>
+        <v>3.97</v>
       </c>
       <c r="D47" t="n">
         <v>2.97</v>
@@ -2463,7 +2463,7 @@
         <v>112</v>
       </c>
       <c r="C48" t="n">
-        <v>4.2</v>
+        <v>4.67</v>
       </c>
       <c r="D48"/>
       <c r="E48"/>
@@ -2492,7 +2492,7 @@
         <v>114</v>
       </c>
       <c r="C49" t="n">
-        <v>3.17</v>
+        <v>3.3</v>
       </c>
       <c r="D49"/>
       <c r="E49" t="n">
@@ -2525,7 +2525,7 @@
         <v>116</v>
       </c>
       <c r="C50" t="n">
-        <v>3.32</v>
+        <v>3.45</v>
       </c>
       <c r="D50"/>
       <c r="E50"/>
@@ -2554,7 +2554,7 @@
         <v>118</v>
       </c>
       <c r="C51" t="n">
-        <v>3.64</v>
+        <v>3.78</v>
       </c>
       <c r="D51"/>
       <c r="E51" t="n">
@@ -2585,7 +2585,7 @@
         <v>120</v>
       </c>
       <c r="C52" t="n">
-        <v>3.38</v>
+        <v>3.54</v>
       </c>
       <c r="D52"/>
       <c r="E52"/>
@@ -2614,7 +2614,7 @@
         <v>122</v>
       </c>
       <c r="C53" t="n">
-        <v>3.85</v>
+        <v>3.95</v>
       </c>
       <c r="D53" t="n">
         <v>3.42</v>
@@ -2647,7 +2647,7 @@
         <v>124</v>
       </c>
       <c r="C54" t="n">
-        <v>3.42</v>
+        <v>3.56</v>
       </c>
       <c r="D54"/>
       <c r="E54" t="n">
@@ -2678,7 +2678,7 @@
         <v>126</v>
       </c>
       <c r="C55" t="n">
-        <v>3.93</v>
+        <v>4.07</v>
       </c>
       <c r="D55" t="n">
         <v>3.51</v>
@@ -2707,7 +2707,7 @@
         <v>128</v>
       </c>
       <c r="C56" t="n">
-        <v>2.25</v>
+        <v>2.37</v>
       </c>
       <c r="D56" t="n">
         <v>3.75</v>
@@ -2740,7 +2740,7 @@
         <v>130</v>
       </c>
       <c r="C57" t="n">
-        <v>4.33</v>
+        <v>4.46</v>
       </c>
       <c r="D57"/>
       <c r="E57"/>
@@ -2769,7 +2769,7 @@
         <v>132</v>
       </c>
       <c r="C58" t="n">
-        <v>4.47</v>
+        <v>4.58</v>
       </c>
       <c r="D58" t="n">
         <v>3.54</v>
@@ -2798,7 +2798,7 @@
         <v>134</v>
       </c>
       <c r="C59" t="n">
-        <v>3.5</v>
+        <v>3.64</v>
       </c>
       <c r="D59"/>
       <c r="E59" t="n">
@@ -2829,7 +2829,7 @@
         <v>136</v>
       </c>
       <c r="C60" t="n">
-        <v>3.58</v>
+        <v>3.71</v>
       </c>
       <c r="D60"/>
       <c r="E60"/>
@@ -2858,7 +2858,7 @@
         <v>138</v>
       </c>
       <c r="C61" t="n">
-        <v>5.09</v>
+        <v>5.39</v>
       </c>
       <c r="D61" t="n">
         <v>3.66</v>
@@ -2887,7 +2887,7 @@
         <v>140</v>
       </c>
       <c r="C62" t="n">
-        <v>4.68</v>
+        <v>4.85</v>
       </c>
       <c r="D62" t="n">
         <v>3.66</v>
@@ -2920,7 +2920,7 @@
         <v>142</v>
       </c>
       <c r="C63" t="n">
-        <v>3.59</v>
+        <v>3.78</v>
       </c>
       <c r="D63"/>
       <c r="E63" t="n">
@@ -2951,7 +2951,7 @@
         <v>144</v>
       </c>
       <c r="C64" t="n">
-        <v>3.96</v>
+        <v>3.97</v>
       </c>
       <c r="D64"/>
       <c r="E64"/>
@@ -2980,7 +2980,7 @@
         <v>146</v>
       </c>
       <c r="C65" t="n">
-        <v>4.23</v>
+        <v>4.38</v>
       </c>
       <c r="D65" t="n">
         <v>3.87</v>
@@ -3009,7 +3009,7 @@
         <v>148</v>
       </c>
       <c r="C66" t="n">
-        <v>5.29</v>
+        <v>5.33</v>
       </c>
       <c r="D66" t="n">
         <v>3.97</v>
@@ -3038,7 +3038,7 @@
         <v>150</v>
       </c>
       <c r="C67" t="n">
-        <v>4.33</v>
+        <v>4.26</v>
       </c>
       <c r="D67"/>
       <c r="E67"/>
@@ -3067,7 +3067,7 @@
         <v>152</v>
       </c>
       <c r="C68" t="n">
-        <v>4.44</v>
+        <v>4.63</v>
       </c>
       <c r="D68"/>
       <c r="E68" t="n">
@@ -3096,7 +3096,7 @@
         <v>154</v>
       </c>
       <c r="C69" t="n">
-        <v>4.06</v>
+        <v>4.2</v>
       </c>
       <c r="D69"/>
       <c r="E69" t="n">
@@ -3125,7 +3125,7 @@
         <v>156</v>
       </c>
       <c r="C70" t="n">
-        <v>3.31</v>
+        <v>3.46</v>
       </c>
       <c r="D70" t="n">
         <v>4.11</v>
@@ -3154,7 +3154,7 @@
         <v>158</v>
       </c>
       <c r="C71" t="n">
-        <v>4.69</v>
+        <v>4.81</v>
       </c>
       <c r="D71"/>
       <c r="E71" t="n">
@@ -3185,7 +3185,7 @@
         <v>160</v>
       </c>
       <c r="C72" t="n">
-        <v>4.07</v>
+        <v>4.08</v>
       </c>
       <c r="D72"/>
       <c r="E72"/>
@@ -3214,7 +3214,7 @@
         <v>162</v>
       </c>
       <c r="C73" t="n">
-        <v>4.89</v>
+        <v>5</v>
       </c>
       <c r="D73"/>
       <c r="E73"/>
@@ -3243,7 +3243,7 @@
         <v>164</v>
       </c>
       <c r="C74" t="n">
-        <v>5.05</v>
+        <v>4.28</v>
       </c>
       <c r="D74"/>
       <c r="E74"/>
@@ -3272,7 +3272,7 @@
         <v>166</v>
       </c>
       <c r="C75" t="n">
-        <v>4.76</v>
+        <v>4.78</v>
       </c>
       <c r="D75"/>
       <c r="E75" t="n">
@@ -3303,7 +3303,7 @@
         <v>168</v>
       </c>
       <c r="C76" t="n">
-        <v>5.05</v>
+        <v>5.24</v>
       </c>
       <c r="D76"/>
       <c r="E76"/>
@@ -3332,7 +3332,7 @@
         <v>170</v>
       </c>
       <c r="C77" t="n">
-        <v>4.44</v>
+        <v>4.58</v>
       </c>
       <c r="D77"/>
       <c r="E77" t="n">
@@ -3363,7 +3363,7 @@
         <v>172</v>
       </c>
       <c r="C78" t="n">
-        <v>4.8</v>
+        <v>4.46</v>
       </c>
       <c r="D78" t="n">
         <v>4.42</v>
@@ -3398,7 +3398,7 @@
         <v>174</v>
       </c>
       <c r="C79" t="n">
-        <v>4.16</v>
+        <v>4.29</v>
       </c>
       <c r="D79"/>
       <c r="E79"/>
@@ -3427,7 +3427,7 @@
         <v>176</v>
       </c>
       <c r="C80" t="n">
-        <v>4.62</v>
+        <v>4.77</v>
       </c>
       <c r="D80" t="n">
         <v>4.5</v>
@@ -3456,7 +3456,7 @@
         <v>178</v>
       </c>
       <c r="C81" t="n">
-        <v>5.09</v>
+        <v>5.23</v>
       </c>
       <c r="D81"/>
       <c r="E81" t="n">
@@ -3487,7 +3487,7 @@
         <v>180</v>
       </c>
       <c r="C82" t="n">
-        <v>4.98</v>
+        <v>5.16</v>
       </c>
       <c r="D82"/>
       <c r="E82" t="n">
@@ -3516,7 +3516,7 @@
         <v>182</v>
       </c>
       <c r="C83" t="n">
-        <v>5.61</v>
+        <v>5.8</v>
       </c>
       <c r="D83"/>
       <c r="E83"/>
@@ -3545,7 +3545,7 @@
         <v>184</v>
       </c>
       <c r="C84" t="n">
-        <v>4.36</v>
+        <v>4.42</v>
       </c>
       <c r="D84" t="n">
         <v>4.59</v>
@@ -3574,7 +3574,7 @@
         <v>186</v>
       </c>
       <c r="C85" t="n">
-        <v>5.34</v>
+        <v>5.48</v>
       </c>
       <c r="D85"/>
       <c r="E85"/>
@@ -3603,7 +3603,7 @@
         <v>188</v>
       </c>
       <c r="C86" t="n">
-        <v>4.96</v>
+        <v>5.09</v>
       </c>
       <c r="D86"/>
       <c r="E86"/>
@@ -3632,7 +3632,7 @@
         <v>190</v>
       </c>
       <c r="C87" t="n">
-        <v>5.41</v>
+        <v>5.49</v>
       </c>
       <c r="D87"/>
       <c r="E87"/>
@@ -3661,7 +3661,7 @@
         <v>192</v>
       </c>
       <c r="C88" t="n">
-        <v>5.65</v>
+        <v>6</v>
       </c>
       <c r="D88"/>
       <c r="E88"/>
@@ -3690,7 +3690,7 @@
         <v>194</v>
       </c>
       <c r="C89" t="n">
-        <v>5.34</v>
+        <v>5.5</v>
       </c>
       <c r="D89"/>
       <c r="E89" t="n">
@@ -3719,7 +3719,7 @@
         <v>196</v>
       </c>
       <c r="C90" t="n">
-        <v>3.66</v>
+        <v>4.07</v>
       </c>
       <c r="D90" t="n">
         <v>4.76</v>
@@ -3748,7 +3748,7 @@
         <v>198</v>
       </c>
       <c r="C91" t="n">
-        <v>3.74</v>
+        <v>3.88</v>
       </c>
       <c r="D91"/>
       <c r="E91"/>
@@ -3777,7 +3777,7 @@
         <v>200</v>
       </c>
       <c r="C92" t="n">
-        <v>5.73</v>
+        <v>5.87</v>
       </c>
       <c r="D92" t="n">
         <v>4.88</v>
@@ -3806,7 +3806,7 @@
         <v>202</v>
       </c>
       <c r="C93" t="n">
-        <v>5.52</v>
+        <v>5.68</v>
       </c>
       <c r="D93"/>
       <c r="E93"/>
@@ -3835,7 +3835,7 @@
         <v>204</v>
       </c>
       <c r="C94" t="n">
-        <v>5.97</v>
+        <v>6.12</v>
       </c>
       <c r="D94" t="n">
         <v>5.17</v>
@@ -3864,7 +3864,7 @@
         <v>206</v>
       </c>
       <c r="C95" t="n">
-        <v>5.84</v>
+        <v>5.97</v>
       </c>
       <c r="D95"/>
       <c r="E95"/>
@@ -3922,7 +3922,7 @@
         <v>210</v>
       </c>
       <c r="C97" t="n">
-        <v>6.07</v>
+        <v>6.24</v>
       </c>
       <c r="D97"/>
       <c r="E97" t="n">
@@ -3953,7 +3953,7 @@
         <v>212</v>
       </c>
       <c r="C98" t="n">
-        <v>6.29</v>
+        <v>6.3</v>
       </c>
       <c r="D98"/>
       <c r="E98"/>
@@ -3982,7 +3982,7 @@
         <v>214</v>
       </c>
       <c r="C99" t="n">
-        <v>7.23</v>
+        <v>7.37</v>
       </c>
       <c r="D99"/>
       <c r="E99" t="n">
@@ -4013,7 +4013,7 @@
         <v>216</v>
       </c>
       <c r="C100" t="n">
-        <v>8.54</v>
+        <v>8.72</v>
       </c>
       <c r="D100" t="n">
         <v>7.15</v>
@@ -4042,7 +4042,7 @@
         <v>218</v>
       </c>
       <c r="C101" t="n">
-        <v>8.04</v>
+        <v>8.07</v>
       </c>
       <c r="D101" t="n">
         <v>7.27</v>

</xml_diff>